<commit_message>
added TEM images for manual data analysis later to be incorporated in deep learning algorithm
</commit_message>
<xml_diff>
--- a/ptxdiffconc.xlsx
+++ b/ptxdiffconc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Feroze\Google Drive\DUKE 2016-2020\AxoSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C47ADB-2B74-4DE8-A8C2-6AD4AFC3C1CF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7873B007-1032-42C0-85A9-1044C6E4E6C2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="7932" xr2:uid="{7C8E119D-E43A-48DC-A79E-D87DB8623B38}"/>
   </bookViews>
@@ -30,10 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
-  <si>
-    <t>File</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="9">
   <si>
     <t>Amplitude</t>
   </si>
@@ -41,175 +38,25 @@
     <t>Scaled NCV</t>
   </si>
   <si>
-    <t>Ptx 100nM 1.1.1.txt</t>
+    <t>Group</t>
   </si>
   <si>
-    <t>Ptx 100nM 1.1.2.txt</t>
+    <t>ctrl</t>
   </si>
   <si>
-    <t>Ptx 100nM 1.1.3.txt</t>
+    <t>ptx 100nM</t>
   </si>
   <si>
-    <t>Ptx 100nM 1.1.4.txt</t>
+    <t>ptx 10nM</t>
   </si>
   <si>
-    <t>Ptx 100nM 1.2.1.txt</t>
+    <t>ptx 150nM</t>
   </si>
   <si>
-    <t>Ptx 100nM 1.2.2.txt</t>
+    <t>ptx 1nM</t>
   </si>
   <si>
-    <t>Ptx 100nM 1.2.3.txt</t>
-  </si>
-  <si>
-    <t>Ptx 100nM 1.2.4.txt</t>
-  </si>
-  <si>
-    <t>Ptx 100nM 2.1.1.txt</t>
-  </si>
-  <si>
-    <t>Ptx 100nM 2.1.2.txt</t>
-  </si>
-  <si>
-    <t>Ptx 100nM 2.1.3.txt</t>
-  </si>
-  <si>
-    <t>Ptx 100nM 2.2.1.txt</t>
-  </si>
-  <si>
-    <t>Ptx 100nM 2.2.2.txt</t>
-  </si>
-  <si>
-    <t>Ptx 100nM 2.2.3.txt</t>
-  </si>
-  <si>
-    <t>Ptx 200nM 1.1.1.txt</t>
-  </si>
-  <si>
-    <t>Ptx 200nM 1.1.2.txt</t>
-  </si>
-  <si>
-    <t>Ptx 200nM 1.1.3.txt</t>
-  </si>
-  <si>
-    <t>Ptx 200nM 1.1.4.txt</t>
-  </si>
-  <si>
-    <t>Ptx 200nM 1.2.1.txt</t>
-  </si>
-  <si>
-    <t>Ptx 200nM 1.2.2.txt</t>
-  </si>
-  <si>
-    <t>Ptx 200nM 1.2.3.txt</t>
-  </si>
-  <si>
-    <t>Ptx 200nM 2.1.1.txt</t>
-  </si>
-  <si>
-    <t>Ptx 200nM 2.1.2.txt</t>
-  </si>
-  <si>
-    <t>Ptx 200nM 2.1.3.txt</t>
-  </si>
-  <si>
-    <t>Ptx 200nM 2.1.4.txt</t>
-  </si>
-  <si>
-    <t>Ptx 200nM 2.2.1.txt</t>
-  </si>
-  <si>
-    <t>Ptx 200nM 2.2.2.txt</t>
-  </si>
-  <si>
-    <t>Ptx 200nM 2.2.3.txt</t>
-  </si>
-  <si>
-    <t>Ptx 50nM 1.1.1.txt</t>
-  </si>
-  <si>
-    <t>Ptx 50nM 1.1.2.txt</t>
-  </si>
-  <si>
-    <t>Ptx 50nM 1.1.3.txt</t>
-  </si>
-  <si>
-    <t>Ptx 50nM 1.1.4.txt</t>
-  </si>
-  <si>
-    <t>Ptx 50nM 1.2.1.txt</t>
-  </si>
-  <si>
-    <t>Ptx 50nM 1.2.2.txt</t>
-  </si>
-  <si>
-    <t>Ptx 50nM 1.2.3.txt</t>
-  </si>
-  <si>
-    <t>Ptx 50nM 1.2.4.txt</t>
-  </si>
-  <si>
-    <t>Ptx 50nM 2.1.1.txt</t>
-  </si>
-  <si>
-    <t>Ptx 50nM 2.1.2.txt</t>
-  </si>
-  <si>
-    <t>Ptx 50nM 2.1.3.txt</t>
-  </si>
-  <si>
-    <t>Ptx 50nM 2.1.4.txt</t>
-  </si>
-  <si>
-    <t>Ptx 50nM 2.2.1.txt</t>
-  </si>
-  <si>
-    <t>ctrl 1.1.1.txt</t>
-  </si>
-  <si>
-    <t>ctrl 1.1.2.txt</t>
-  </si>
-  <si>
-    <t>ctrl 1.1.3.txt</t>
-  </si>
-  <si>
-    <t>ctrl 1.1.4.txt</t>
-  </si>
-  <si>
-    <t>ctrl 1.2.1.txt</t>
-  </si>
-  <si>
-    <t>ctrl 1.2.2.txt</t>
-  </si>
-  <si>
-    <t>ctrl 1.2.3.txt</t>
-  </si>
-  <si>
-    <t>ctrl 1.2.4.txt</t>
-  </si>
-  <si>
-    <t>ctrl 2.1.1.txt</t>
-  </si>
-  <si>
-    <t>ctrl 2.1.2.txt</t>
-  </si>
-  <si>
-    <t>ctrl 2.1.3.txt</t>
-  </si>
-  <si>
-    <t>ctrl 2.1.4.txt</t>
-  </si>
-  <si>
-    <t>ctrl 2.2.1.txt</t>
-  </si>
-  <si>
-    <t>ctrl 2.2.2.txt</t>
-  </si>
-  <si>
-    <t>ctrl 2.2.3.txt</t>
-  </si>
-  <si>
-    <t>ctrl 2.2.4.txt</t>
+    <t>ptx 200nM</t>
   </si>
 </sst>
 </file>
@@ -561,23 +408,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69CF060E-16C0-45EF-9C8D-C01CC13BD142}">
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C204"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C58"/>
+      <selection sqref="A1:C204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -585,620 +432,2232 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>5.5922000000000001</v>
+        <v>0.78193999999999997</v>
       </c>
       <c r="C2">
-        <v>3.6101000000000002E-3</v>
+        <v>5.9172000000000001E-3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>3.6215999999999999</v>
+        <v>4.7279999999999998</v>
       </c>
       <c r="C3">
-        <v>6.7568000000000003E-3</v>
+        <v>8.7718999999999991E-3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>2.15</v>
+        <v>1.0212000000000001</v>
       </c>
       <c r="C4">
-        <v>3.4602000000000001E-3</v>
+        <v>5.3476000000000001E-3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>3.9113000000000002</v>
+        <v>2.3649</v>
       </c>
       <c r="C5">
-        <v>7.7518999999999999E-3</v>
+        <v>9.1742999999999998E-3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>1.4603999999999999</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="C6">
-        <v>4.7847000000000002E-3</v>
+        <v>4.0816000000000003E-3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B7">
-        <v>5.1855000000000002</v>
+        <v>1.869</v>
       </c>
       <c r="C7">
-        <v>8.3333000000000001E-3</v>
+        <v>1.0753E-2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B8">
-        <v>0.80286000000000002</v>
+        <v>5.3819999999999997</v>
       </c>
       <c r="C8">
-        <v>6.8966000000000001E-3</v>
+        <v>6.4516E-3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B9">
-        <v>0.76153999999999999</v>
+        <v>8.0268999999999995</v>
       </c>
       <c r="C9">
-        <v>1.1364000000000001E-2</v>
+        <v>1.5873000000000002E-2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B10">
-        <v>3.0545</v>
+        <v>3.6932</v>
       </c>
       <c r="C10">
-        <v>1.1764999999999999E-2</v>
+        <v>6.6224999999999999E-3</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B11">
-        <v>3.5</v>
+        <v>1.4067000000000001</v>
       </c>
       <c r="C11">
-        <v>4.2918000000000001E-3</v>
+        <v>1.5384999999999999E-2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B12">
-        <v>0.93181999999999998</v>
+        <v>0.74422999999999995</v>
       </c>
       <c r="C12">
-        <v>1.0101000000000001E-2</v>
+        <v>7.3528999999999999E-3</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B13">
-        <v>4.2042000000000002</v>
+        <v>2.1949000000000001</v>
       </c>
       <c r="C13">
-        <v>7.3528999999999999E-3</v>
+        <v>1.2987E-2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B14">
-        <v>1.5760000000000001</v>
+        <v>1.18</v>
       </c>
       <c r="C14">
-        <v>2.7623999999999999E-3</v>
+        <v>5.6179999999999997E-3</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B15">
-        <v>1.0412999999999999</v>
+        <v>4.7469000000000001</v>
       </c>
       <c r="C15">
-        <v>7.0921999999999999E-3</v>
+        <v>1.0869999999999999E-2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="B16">
-        <v>1.4638</v>
+        <v>0.95365999999999995</v>
       </c>
       <c r="C16">
-        <v>2.2989E-3</v>
+        <v>5.1282000000000003E-3</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="B17">
-        <v>1.1639999999999999</v>
+        <v>4.2706</v>
       </c>
       <c r="C17">
-        <v>6.3290999999999998E-3</v>
+        <v>1.3889E-2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B18">
-        <v>0.64</v>
+        <v>10.29</v>
       </c>
       <c r="C18">
-        <v>3.4014000000000002E-3</v>
+        <v>6.8027000000000001E-3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="B19">
-        <v>1.5780000000000001</v>
+        <v>4.2544000000000004</v>
       </c>
       <c r="C19">
-        <v>9.1742999999999998E-3</v>
+        <v>1.7544000000000001E-2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B20">
-        <v>1.4724999999999999</v>
+        <v>0.87878999999999996</v>
       </c>
       <c r="C20">
-        <v>5.9524000000000001E-3</v>
+        <v>6.9443999999999999E-3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="B21">
-        <v>0.90980000000000005</v>
+        <v>5.3159000000000001</v>
       </c>
       <c r="C21">
-        <v>8.6207000000000002E-3</v>
+        <v>1.0309E-2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="B22">
-        <v>2.3096000000000001</v>
+        <v>5.3681000000000001</v>
       </c>
       <c r="C22">
-        <v>0.01</v>
+        <v>5.0251000000000002E-3</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="B23">
-        <v>0.86307999999999996</v>
+        <v>1.7171000000000001</v>
       </c>
       <c r="C23">
-        <v>4.9505E-3</v>
+        <v>1.7857000000000001E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B24">
-        <v>3.3069999999999999</v>
+        <v>3.0973000000000002</v>
       </c>
       <c r="C24">
-        <v>9.1742999999999998E-3</v>
+        <v>4.5455000000000001E-3</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="B25">
-        <v>0.9</v>
+        <v>2.0811999999999999</v>
       </c>
       <c r="C25">
-        <v>4.1666999999999997E-3</v>
+        <v>1.2658000000000001E-2</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="B26">
-        <v>4.7350000000000003</v>
+        <v>5.9189999999999996</v>
       </c>
       <c r="C26">
-        <v>1.1764999999999999E-2</v>
+        <v>1.1235999999999999E-2</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="B27">
-        <v>3.2837999999999998</v>
+        <v>3.3346</v>
       </c>
       <c r="C27">
-        <v>8.3333000000000001E-3</v>
+        <v>1.0204E-2</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="B28">
-        <v>0.55323</v>
+        <v>1.9196</v>
       </c>
       <c r="C28">
-        <v>1.0753E-2</v>
+        <v>9.8039000000000008E-3</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B29">
-        <v>1.1308</v>
+        <v>2.2646999999999999</v>
       </c>
       <c r="C29">
-        <v>5.2632E-3</v>
+        <v>1.2987E-2</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="B30">
-        <v>0.92240999999999995</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="C30">
-        <v>4.6296000000000002E-3</v>
+        <v>4.5249000000000001E-3</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>3</v>
+      </c>
+      <c r="B31">
+        <v>2.1299000000000001</v>
+      </c>
+      <c r="C31">
+        <v>1.1905000000000001E-2</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="B32">
-        <v>1.1093999999999999</v>
+        <v>2.9087999999999998</v>
       </c>
       <c r="C32">
-        <v>4.3290000000000004E-3</v>
+        <v>6.4102999999999999E-3</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="B33">
-        <v>3.9660000000000002</v>
+        <v>6.1157000000000004</v>
       </c>
       <c r="C33">
-        <v>7.6335999999999999E-3</v>
+        <v>1.5152000000000001E-2</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="B34">
-        <v>0.97450999999999999</v>
+        <v>4.9154</v>
       </c>
       <c r="C34">
-        <v>3.8462000000000001E-3</v>
+        <v>4.7169999999999998E-3</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="B35">
-        <v>3.0491000000000001</v>
+        <v>5.4179000000000004</v>
       </c>
       <c r="C35">
-        <v>1.1235999999999999E-2</v>
+        <v>1.6129000000000001E-2</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="B36">
-        <v>1.7632000000000001</v>
+        <v>142.31200000000001</v>
       </c>
       <c r="C36">
-        <v>4.4444000000000003E-3</v>
+        <v>1.6129000000000001E-2</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="B37">
-        <v>6.2607999999999997</v>
+        <v>4.8765000000000001</v>
       </c>
       <c r="C37">
-        <v>7.6335999999999999E-3</v>
+        <v>1.3889E-2</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="B38">
-        <v>2.6602999999999999</v>
+        <v>185.178</v>
       </c>
       <c r="C38">
-        <v>4.2553000000000001E-3</v>
+        <v>8.3333000000000001E-3</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="B39">
-        <v>4.6859999999999999</v>
+        <v>2.34</v>
       </c>
       <c r="C39">
-        <v>8.4746000000000005E-3</v>
+        <v>9.3457999999999996E-3</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="B40">
-        <v>2.1722000000000001</v>
+        <v>146.26920000000001</v>
       </c>
       <c r="C40">
-        <v>3.9062999999999997E-3</v>
+        <v>9.6153999999999996E-3</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="B41">
-        <v>1.4204000000000001</v>
+        <v>2.2153999999999998</v>
       </c>
       <c r="C41">
-        <v>6.7568000000000003E-3</v>
+        <v>9.2592999999999998E-3</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="B42">
-        <v>3.0464000000000002</v>
+        <v>152.1019</v>
       </c>
       <c r="C42">
-        <v>6.9443999999999999E-3</v>
+        <v>1.2500000000000001E-2</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="B43">
-        <v>0.88036000000000003</v>
+        <v>179.6679</v>
       </c>
       <c r="C43">
-        <v>7.1942000000000004E-3</v>
+        <v>1.1235999999999999E-2</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="B44">
-        <v>10.618600000000001</v>
+        <v>200.23</v>
       </c>
       <c r="C44">
-        <v>1.1235999999999999E-2</v>
+        <v>1.4493000000000001E-2</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="B45">
-        <v>19.220800000000001</v>
+        <v>2.2462</v>
       </c>
       <c r="C45">
-        <v>6.8493E-3</v>
+        <v>9.0909000000000007E-3</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="B46">
-        <v>7.7221000000000002</v>
+        <v>3.2414999999999998</v>
       </c>
       <c r="C46">
-        <v>6.5358999999999999E-3</v>
+        <v>3.1250000000000002E-3</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="B47">
-        <v>5.6932</v>
+        <v>1.2096</v>
       </c>
       <c r="C47">
-        <v>5.6179999999999997E-3</v>
+        <v>1.0101000000000001E-2</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="B48">
-        <v>4.2854999999999999</v>
+        <v>0.74422999999999995</v>
       </c>
       <c r="C48">
-        <v>6.4102999999999999E-3</v>
+        <v>2.4631000000000002E-3</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="B49">
-        <v>0.77692000000000005</v>
+        <v>3.3075000000000001</v>
       </c>
       <c r="C49">
-        <v>1.5698999999999999E-3</v>
+        <v>5.1812999999999998E-3</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="B50">
-        <v>9.2609999999999992</v>
+        <v>0.45546999999999999</v>
       </c>
       <c r="C50">
-        <v>9.9010000000000001E-3</v>
+        <v>6.2893000000000003E-3</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="B51">
-        <v>3.6579999999999999</v>
+        <v>0.75600000000000001</v>
       </c>
       <c r="C51">
-        <v>3.5336E-3</v>
+        <v>7.8740000000000008E-3</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="B52">
-        <v>3.5362</v>
+        <v>8.9571000000000005</v>
       </c>
       <c r="C52">
-        <v>9.9010000000000001E-3</v>
+        <v>2.7932999999999999E-3</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>54</v>
+        <v>3</v>
       </c>
       <c r="B53">
-        <v>0.70833000000000002</v>
+        <v>2.58</v>
       </c>
       <c r="C53">
-        <v>4.8544E-3</v>
+        <v>1.0753E-2</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="B54">
-        <v>4.8339999999999996</v>
+        <v>1.8692</v>
       </c>
       <c r="C54">
-        <v>8.0000000000000002E-3</v>
+        <v>1.0526000000000001E-2</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="B55">
-        <v>1.4518</v>
+        <v>0.61624999999999996</v>
       </c>
       <c r="C55">
-        <v>3.6495999999999998E-3</v>
+        <v>4.6083000000000001E-3</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="B56">
-        <v>1.0662</v>
+        <v>4.7619999999999996</v>
       </c>
       <c r="C56">
-        <v>1.2194999999999999E-2</v>
+        <v>8.1300999999999995E-3</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>58</v>
+        <v>3</v>
       </c>
       <c r="B57">
-        <v>2.8384</v>
+        <v>1.2455000000000001</v>
       </c>
       <c r="C57">
-        <v>4.6728999999999998E-3</v>
+        <v>6.3693999999999999E-3</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="B58">
-        <v>3.6246</v>
+        <v>4.2774000000000001</v>
       </c>
       <c r="C58">
+        <v>9.6153999999999996E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59">
+        <v>0.90678000000000003</v>
+      </c>
+      <c r="C59">
+        <v>7.6923E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" t="s">
+        <v>3</v>
+      </c>
+      <c r="B60">
+        <v>3.5059</v>
+      </c>
+      <c r="C60">
+        <v>1.1627999999999999E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" t="s">
+        <v>3</v>
+      </c>
+      <c r="B61">
+        <v>0.57418999999999998</v>
+      </c>
+      <c r="C61">
+        <v>6.0241000000000001E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" t="s">
+        <v>3</v>
+      </c>
+      <c r="B62">
+        <v>1.6552</v>
+      </c>
+      <c r="C62">
+        <v>7.2992999999999999E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" t="s">
+        <v>3</v>
+      </c>
+      <c r="B63">
+        <v>1.3090999999999999</v>
+      </c>
+      <c r="C63">
+        <v>4.5662000000000003E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" t="s">
+        <v>3</v>
+      </c>
+      <c r="B64">
+        <v>3.5480999999999998</v>
+      </c>
+      <c r="C64">
+        <v>1.1110999999999999E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" t="s">
+        <v>3</v>
+      </c>
+      <c r="B65">
+        <v>1.2222</v>
+      </c>
+      <c r="C65">
+        <v>5.4348E-3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66">
+        <v>6.1379999999999999</v>
+      </c>
+      <c r="C66">
+        <v>8.6957000000000007E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" t="s">
+        <v>3</v>
+      </c>
+      <c r="B67">
+        <v>0.96028999999999998</v>
+      </c>
+      <c r="C67">
+        <v>1.0989000000000001E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" t="s">
+        <v>3</v>
+      </c>
+      <c r="B68">
+        <v>3.8942999999999999</v>
+      </c>
+      <c r="C68">
+        <v>1.9231000000000002E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" t="s">
+        <v>3</v>
+      </c>
+      <c r="B69">
+        <v>0.7</v>
+      </c>
+      <c r="C69">
+        <v>5.5249000000000001E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" t="s">
+        <v>3</v>
+      </c>
+      <c r="B70">
+        <v>1.2579</v>
+      </c>
+      <c r="C70">
+        <v>1.7544000000000001E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" t="s">
+        <v>3</v>
+      </c>
+      <c r="B71">
+        <v>1.1359999999999999</v>
+      </c>
+      <c r="C71">
+        <v>6.5789000000000004E-3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" t="s">
+        <v>3</v>
+      </c>
+      <c r="B72">
+        <v>7.9158999999999997</v>
+      </c>
+      <c r="C72">
+        <v>7.7518999999999999E-3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" t="s">
+        <v>3</v>
+      </c>
+      <c r="B73">
+        <v>0.98511000000000004</v>
+      </c>
+      <c r="C73">
+        <v>9.3457999999999996E-3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" t="s">
+        <v>3</v>
+      </c>
+      <c r="B74">
+        <v>3.8054000000000001</v>
+      </c>
+      <c r="C74">
+        <v>1.0204E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" t="s">
+        <v>3</v>
+      </c>
+      <c r="B75">
+        <v>0.57777999999999996</v>
+      </c>
+      <c r="C75">
+        <v>3.9683000000000001E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" t="s">
+        <v>3</v>
+      </c>
+      <c r="B76">
+        <v>3.6659999999999999</v>
+      </c>
+      <c r="C76">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" t="s">
+        <v>4</v>
+      </c>
+      <c r="B77">
+        <v>4.24</v>
+      </c>
+      <c r="C77">
+        <v>7.5757999999999997E-3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" t="s">
+        <v>4</v>
+      </c>
+      <c r="B78">
+        <v>1.9295</v>
+      </c>
+      <c r="C78">
+        <v>4.5662000000000003E-3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" t="s">
+        <v>4</v>
+      </c>
+      <c r="B79">
+        <v>0.69411999999999996</v>
+      </c>
+      <c r="C79">
+        <v>5.2356E-3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" t="s">
+        <v>4</v>
+      </c>
+      <c r="B80">
+        <v>1.1868000000000001</v>
+      </c>
+      <c r="C80">
+        <v>8.1300999999999995E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" t="s">
+        <v>4</v>
+      </c>
+      <c r="B81">
+        <v>0.85070000000000001</v>
+      </c>
+      <c r="C81">
+        <v>3.3557000000000001E-3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" t="s">
+        <v>4</v>
+      </c>
+      <c r="B82">
+        <v>3.6364999999999998</v>
+      </c>
+      <c r="C82">
+        <v>9.4339999999999997E-3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" t="s">
+        <v>4</v>
+      </c>
+      <c r="B83">
+        <v>0.84528000000000003</v>
+      </c>
+      <c r="C83">
+        <v>3.3333E-3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" t="s">
+        <v>4</v>
+      </c>
+      <c r="B84">
+        <v>2.7475000000000001</v>
+      </c>
+      <c r="C84">
+        <v>8.6957000000000007E-3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" t="s">
+        <v>4</v>
+      </c>
+      <c r="B85">
+        <v>5.2122000000000002</v>
+      </c>
+      <c r="C85">
+        <v>6.2112000000000001E-3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" t="s">
+        <v>4</v>
+      </c>
+      <c r="B86">
+        <v>2.5114999999999998</v>
+      </c>
+      <c r="C86">
+        <v>6.1728E-3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87" t="s">
+        <v>4</v>
+      </c>
+      <c r="B87">
+        <v>441.93</v>
+      </c>
+      <c r="C87">
+        <v>9.0909000000000007E-3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A88" t="s">
+        <v>4</v>
+      </c>
+      <c r="B88">
+        <v>0.89400000000000002</v>
+      </c>
+      <c r="C88">
+        <v>6.7568000000000003E-3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89" t="s">
+        <v>4</v>
+      </c>
+      <c r="B89">
+        <v>0.76037999999999994</v>
+      </c>
+      <c r="C89">
+        <v>3.0303000000000001E-3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90" t="s">
+        <v>4</v>
+      </c>
+      <c r="B90">
+        <v>2.0019999999999998</v>
+      </c>
+      <c r="C90">
+        <v>8.4034000000000001E-3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91" t="s">
+        <v>4</v>
+      </c>
+      <c r="B91">
+        <v>192.232</v>
+      </c>
+      <c r="C91">
+        <v>8.3333000000000001E-3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92" t="s">
+        <v>5</v>
+      </c>
+      <c r="B92">
+        <v>1</v>
+      </c>
+      <c r="C92">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93" t="s">
+        <v>5</v>
+      </c>
+      <c r="B93">
+        <v>3.9161000000000001</v>
+      </c>
+      <c r="C93">
+        <v>7.5757999999999997E-3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94" t="s">
+        <v>5</v>
+      </c>
+      <c r="B94">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="C94">
+        <v>5.0761000000000001E-3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95" t="s">
+        <v>5</v>
+      </c>
+      <c r="B95">
+        <v>3.278</v>
+      </c>
+      <c r="C95">
+        <v>7.7518999999999999E-3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96" t="s">
+        <v>5</v>
+      </c>
+      <c r="B96">
+        <v>2.1089000000000002</v>
+      </c>
+      <c r="C96">
         <v>7.9365000000000008E-3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97" t="s">
+        <v>5</v>
+      </c>
+      <c r="B97">
+        <v>2.1381000000000001</v>
+      </c>
+      <c r="C97">
+        <v>8.6957000000000007E-3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98" t="s">
+        <v>5</v>
+      </c>
+      <c r="B98">
+        <v>3.1760000000000002</v>
+      </c>
+      <c r="C98">
+        <v>6.6224999999999999E-3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99" t="s">
+        <v>5</v>
+      </c>
+      <c r="B99">
+        <v>155.2097</v>
+      </c>
+      <c r="C99">
+        <v>1.2194999999999999E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100" t="s">
+        <v>5</v>
+      </c>
+      <c r="B100">
+        <v>0.98678999999999994</v>
+      </c>
+      <c r="C100">
+        <v>3.9215999999999999E-3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101" t="s">
+        <v>5</v>
+      </c>
+      <c r="B101">
+        <v>4.8185000000000002</v>
+      </c>
+      <c r="C101">
+        <v>1.1627999999999999E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A102" t="s">
+        <v>5</v>
+      </c>
+      <c r="B102">
+        <v>1.8269</v>
+      </c>
+      <c r="C102">
+        <v>3.5971000000000002E-3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A103" t="s">
+        <v>5</v>
+      </c>
+      <c r="B103">
+        <v>5.86</v>
+      </c>
+      <c r="C103">
+        <v>1.1627999999999999E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A104" t="s">
+        <v>6</v>
+      </c>
+      <c r="B104">
+        <v>1.3150999999999999</v>
+      </c>
+      <c r="C104">
+        <v>4.9261000000000001E-3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A105" t="s">
+        <v>6</v>
+      </c>
+      <c r="B105">
+        <v>3.8961999999999999</v>
+      </c>
+      <c r="C105">
+        <v>8.1300999999999995E-3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A106" t="s">
+        <v>6</v>
+      </c>
+      <c r="B106">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="C106">
+        <v>6.6667000000000002E-3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A107" t="s">
+        <v>6</v>
+      </c>
+      <c r="B107">
+        <v>1.9466000000000001</v>
+      </c>
+      <c r="C107">
+        <v>1.7857000000000001E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A108" t="s">
+        <v>6</v>
+      </c>
+      <c r="B108">
+        <v>3.5076999999999998</v>
+      </c>
+      <c r="C108">
+        <v>1.0309E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A109" t="s">
+        <v>6</v>
+      </c>
+      <c r="B109">
+        <v>6.1231999999999998</v>
+      </c>
+      <c r="C109">
+        <v>1.7240999999999999E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A110" t="s">
+        <v>6</v>
+      </c>
+      <c r="B110">
+        <v>1.3118000000000001</v>
+      </c>
+      <c r="C110">
+        <v>4.2193999999999999E-3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A111" t="s">
+        <v>6</v>
+      </c>
+      <c r="B111">
+        <v>5.6630000000000003</v>
+      </c>
+      <c r="C111">
+        <v>1.5873000000000002E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A112" t="s">
+        <v>6</v>
+      </c>
+      <c r="B112">
+        <v>0.89817999999999998</v>
+      </c>
+      <c r="C112">
+        <v>8.6957000000000007E-3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A113" t="s">
+        <v>6</v>
+      </c>
+      <c r="B113">
+        <v>3.9590000000000001</v>
+      </c>
+      <c r="C113">
+        <v>1.1110999999999999E-2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A114" t="s">
+        <v>6</v>
+      </c>
+      <c r="B114">
+        <v>1.7578</v>
+      </c>
+      <c r="C114">
+        <v>6.4516E-3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A115" t="s">
+        <v>6</v>
+      </c>
+      <c r="B115">
+        <v>6.8181000000000003</v>
+      </c>
+      <c r="C115">
+        <v>1.2194999999999999E-2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A116" t="s">
+        <v>6</v>
+      </c>
+      <c r="B116">
+        <v>2.4279000000000002</v>
+      </c>
+      <c r="C116">
+        <v>3.4965E-3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A117" t="s">
+        <v>6</v>
+      </c>
+      <c r="B117">
+        <v>4.7145000000000001</v>
+      </c>
+      <c r="C117">
+        <v>1.0526000000000001E-2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A118" t="s">
+        <v>6</v>
+      </c>
+      <c r="B118">
+        <v>0.60192000000000001</v>
+      </c>
+      <c r="C118">
+        <v>9.1742999999999998E-3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A119" t="s">
+        <v>6</v>
+      </c>
+      <c r="B119">
+        <v>5.09</v>
+      </c>
+      <c r="C119">
+        <v>1.2500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A120" t="s">
+        <v>7</v>
+      </c>
+      <c r="B120">
+        <v>173.98429999999999</v>
+      </c>
+      <c r="C120">
+        <v>2.8570999999999999E-2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A121" t="s">
+        <v>7</v>
+      </c>
+      <c r="B121">
+        <v>1.228</v>
+      </c>
+      <c r="C121">
+        <v>1.1364000000000001E-2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A122" t="s">
+        <v>7</v>
+      </c>
+      <c r="B122">
+        <v>4.0557999999999996</v>
+      </c>
+      <c r="C122">
+        <v>5.2356E-3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A123" t="s">
+        <v>7</v>
+      </c>
+      <c r="B123">
+        <v>2.4527000000000001</v>
+      </c>
+      <c r="C123">
+        <v>8.6207000000000002E-3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A124" t="s">
+        <v>7</v>
+      </c>
+      <c r="B124">
+        <v>1.0698000000000001</v>
+      </c>
+      <c r="C124">
+        <v>3.6765000000000001E-3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A125" t="s">
+        <v>7</v>
+      </c>
+      <c r="B125">
+        <v>4.2417999999999996</v>
+      </c>
+      <c r="C125">
+        <v>7.2464000000000001E-3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A126" t="s">
+        <v>7</v>
+      </c>
+      <c r="B126">
+        <v>3.2894999999999999</v>
+      </c>
+      <c r="C126">
+        <v>4.0160999999999999E-3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A127" t="s">
+        <v>7</v>
+      </c>
+      <c r="B127">
+        <v>1.9567000000000001</v>
+      </c>
+      <c r="C127">
+        <v>1.1235999999999999E-2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A128" t="s">
+        <v>7</v>
+      </c>
+      <c r="B128">
+        <v>2.6808000000000001</v>
+      </c>
+      <c r="C128">
+        <v>1.9193999999999999E-3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A129" t="s">
+        <v>7</v>
+      </c>
+      <c r="B129">
+        <v>2.1659999999999999</v>
+      </c>
+      <c r="C129">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A130" t="s">
+        <v>7</v>
+      </c>
+      <c r="B130">
+        <v>0.75185000000000002</v>
+      </c>
+      <c r="C130">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A131" t="s">
+        <v>7</v>
+      </c>
+      <c r="B131">
+        <v>4.032</v>
+      </c>
+      <c r="C131">
+        <v>7.6923E-3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A132" t="s">
+        <v>8</v>
+      </c>
+      <c r="B132">
+        <v>1.1657</v>
+      </c>
+      <c r="C132">
+        <v>5.2632E-3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A133" t="s">
+        <v>8</v>
+      </c>
+      <c r="B133">
+        <v>1.4275</v>
+      </c>
+      <c r="C133">
+        <v>1.5873000000000002E-2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A134" t="s">
+        <v>8</v>
+      </c>
+      <c r="B134">
+        <v>1.0405</v>
+      </c>
+      <c r="C134">
+        <v>4.8309E-3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A135" t="s">
+        <v>8</v>
+      </c>
+      <c r="B135">
+        <v>5.5517000000000003</v>
+      </c>
+      <c r="C135">
+        <v>1.0309E-2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A136" t="s">
+        <v>8</v>
+      </c>
+      <c r="B136">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="C136">
+        <v>4.065E-3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A137" t="s">
+        <v>8</v>
+      </c>
+      <c r="B137">
+        <v>2.7639999999999998</v>
+      </c>
+      <c r="C137">
+        <v>1.7544000000000001E-2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A138" t="s">
+        <v>8</v>
+      </c>
+      <c r="B138">
+        <v>0.73462000000000005</v>
+      </c>
+      <c r="C138">
+        <v>3.9062999999999997E-3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A139" t="s">
+        <v>8</v>
+      </c>
+      <c r="B139">
+        <v>1.1480999999999999</v>
+      </c>
+      <c r="C139">
+        <v>6.8966000000000001E-3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A140" t="s">
+        <v>8</v>
+      </c>
+      <c r="B140">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="C140">
+        <v>7.0422999999999996E-3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A141" t="s">
+        <v>8</v>
+      </c>
+      <c r="B141">
+        <v>3.4866999999999999</v>
+      </c>
+      <c r="C141">
+        <v>1.1627999999999999E-2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A142" t="s">
+        <v>8</v>
+      </c>
+      <c r="B142">
+        <v>3.2721</v>
+      </c>
+      <c r="C142">
+        <v>6.7114000000000002E-3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A143" t="s">
+        <v>8</v>
+      </c>
+      <c r="B143">
+        <v>6.5763999999999996</v>
+      </c>
+      <c r="C143">
+        <v>1.3889E-2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A144" t="s">
+        <v>8</v>
+      </c>
+      <c r="B144">
+        <v>2.6962000000000002</v>
+      </c>
+      <c r="C144">
+        <v>4.5249000000000001E-3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A145" t="s">
+        <v>8</v>
+      </c>
+      <c r="B145">
+        <v>9.0896000000000008</v>
+      </c>
+      <c r="C145">
+        <v>1.1494000000000001E-2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A146" t="s">
+        <v>8</v>
+      </c>
+      <c r="B146">
+        <v>4.95</v>
+      </c>
+      <c r="C146">
+        <v>5.5555999999999999E-3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A147" t="s">
+        <v>8</v>
+      </c>
+      <c r="B147">
+        <v>5.9135</v>
+      </c>
+      <c r="C147">
+        <v>1.4706E-2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A148" t="s">
+        <v>8</v>
+      </c>
+      <c r="B148">
+        <v>1.5423</v>
+      </c>
+      <c r="C148">
+        <v>5.2082999999999999E-3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A149" t="s">
+        <v>8</v>
+      </c>
+      <c r="B149">
+        <v>0.73370999999999997</v>
+      </c>
+      <c r="C149">
+        <v>1.3158E-2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A150" t="s">
+        <v>8</v>
+      </c>
+      <c r="B150">
+        <v>0.59258999999999995</v>
+      </c>
+      <c r="C150">
+        <v>4.7847000000000002E-3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A151" t="s">
+        <v>8</v>
+      </c>
+      <c r="B151">
+        <v>1.0589</v>
+      </c>
+      <c r="C151">
+        <v>1.1905000000000001E-2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A152" t="s">
+        <v>8</v>
+      </c>
+      <c r="B152">
+        <v>3.4540999999999999</v>
+      </c>
+      <c r="C152">
+        <v>5.8824000000000003E-3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A153" t="s">
+        <v>8</v>
+      </c>
+      <c r="B153">
+        <v>1.0545</v>
+      </c>
+      <c r="C153">
+        <v>1.9231000000000002E-2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A154" t="s">
+        <v>8</v>
+      </c>
+      <c r="B154">
+        <v>4.7691999999999997</v>
+      </c>
+      <c r="C154">
+        <v>4.8780000000000004E-3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A155" t="s">
+        <v>8</v>
+      </c>
+      <c r="B155">
+        <v>5.2610999999999999</v>
+      </c>
+      <c r="C155">
+        <v>9.2592999999999998E-3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A156" t="s">
+        <v>8</v>
+      </c>
+      <c r="B156">
+        <v>1.6817</v>
+      </c>
+      <c r="C156">
+        <v>3.663E-3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A157" t="s">
+        <v>8</v>
+      </c>
+      <c r="B157">
+        <v>3.2848999999999999</v>
+      </c>
+      <c r="C157">
+        <v>7.8125E-3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A158" t="s">
+        <v>8</v>
+      </c>
+      <c r="B158">
+        <v>1.9836</v>
+      </c>
+      <c r="C158">
+        <v>3.5842000000000001E-3</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A159" t="s">
+        <v>8</v>
+      </c>
+      <c r="B159">
+        <v>5.1737000000000002</v>
+      </c>
+      <c r="C159">
+        <v>8.1300999999999995E-3</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A160" t="s">
+        <v>8</v>
+      </c>
+      <c r="B160">
+        <v>1.6468</v>
+      </c>
+      <c r="C160">
+        <v>3.8314E-3</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A161" t="s">
+        <v>8</v>
+      </c>
+      <c r="B161">
+        <v>5.0236999999999998</v>
+      </c>
+      <c r="C161">
+        <v>1.5625E-2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A162" t="s">
+        <v>8</v>
+      </c>
+      <c r="B162">
+        <v>2.0392000000000001</v>
+      </c>
+      <c r="C162">
+        <v>6.2112000000000001E-3</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A163" t="s">
+        <v>8</v>
+      </c>
+      <c r="B163">
+        <v>3.7136999999999998</v>
+      </c>
+      <c r="C163">
+        <v>1.0753E-2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A164" t="s">
+        <v>8</v>
+      </c>
+      <c r="B164">
+        <v>0.99922</v>
+      </c>
+      <c r="C164">
+        <v>4.6512000000000003E-3</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A165" t="s">
+        <v>8</v>
+      </c>
+      <c r="B165">
+        <v>2.5194999999999999</v>
+      </c>
+      <c r="C165">
+        <v>9.8039000000000008E-3</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A166" t="s">
+        <v>8</v>
+      </c>
+      <c r="B166">
+        <v>0.95962000000000003</v>
+      </c>
+      <c r="C166">
+        <v>1.0204E-2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A167" t="s">
+        <v>8</v>
+      </c>
+      <c r="B167">
+        <v>0.70286000000000004</v>
+      </c>
+      <c r="C167">
+        <v>5.6817999999999999E-3</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A168" t="s">
+        <v>8</v>
+      </c>
+      <c r="B168">
+        <v>2.5569000000000002</v>
+      </c>
+      <c r="C168">
+        <v>9.2592999999999998E-3</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A169" t="s">
+        <v>8</v>
+      </c>
+      <c r="B169">
+        <v>2.1677</v>
+      </c>
+      <c r="C169">
+        <v>3.3333E-3</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A170" t="s">
+        <v>8</v>
+      </c>
+      <c r="B170">
+        <v>1.1434</v>
+      </c>
+      <c r="C170">
+        <v>4.8076999999999998E-3</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A171" t="s">
+        <v>8</v>
+      </c>
+      <c r="B171">
+        <v>2.004</v>
+      </c>
+      <c r="C171">
+        <v>1.0638E-2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A172" t="s">
+        <v>8</v>
+      </c>
+      <c r="B172">
+        <v>2.4361000000000002</v>
+      </c>
+      <c r="C172">
+        <v>2.8736E-3</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A173" t="s">
+        <v>8</v>
+      </c>
+      <c r="B173">
+        <v>1.6459999999999999</v>
+      </c>
+      <c r="C173">
+        <v>1.0638E-2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A174" t="s">
+        <v>8</v>
+      </c>
+      <c r="B174">
+        <v>0.438</v>
+      </c>
+      <c r="C174">
+        <v>5.2909999999999997E-3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A175" t="s">
+        <v>8</v>
+      </c>
+      <c r="B175">
+        <v>1.8797999999999999</v>
+      </c>
+      <c r="C175">
+        <v>7.4073999999999997E-3</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A176" t="s">
+        <v>8</v>
+      </c>
+      <c r="B176">
+        <v>1.974</v>
+      </c>
+      <c r="C176">
+        <v>3.8462000000000001E-3</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A177" t="s">
+        <v>8</v>
+      </c>
+      <c r="B177">
+        <v>1.3090999999999999</v>
+      </c>
+      <c r="C177">
+        <v>1.1764999999999999E-2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A178" t="s">
+        <v>8</v>
+      </c>
+      <c r="B178">
+        <v>2.1025999999999998</v>
+      </c>
+      <c r="C178">
+        <v>6.2500000000000003E-3</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A179" t="s">
+        <v>8</v>
+      </c>
+      <c r="B179">
+        <v>2.4573999999999998</v>
+      </c>
+      <c r="C179">
+        <v>8.7718999999999991E-3</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A180" t="s">
+        <v>8</v>
+      </c>
+      <c r="B180">
+        <v>0.90532000000000001</v>
+      </c>
+      <c r="C180">
+        <v>3.8760000000000001E-3</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A181" t="s">
+        <v>8</v>
+      </c>
+      <c r="B181">
+        <v>2.1579999999999999</v>
+      </c>
+      <c r="C181">
+        <v>7.6923E-3</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A182" t="s">
+        <v>8</v>
+      </c>
+      <c r="B182">
+        <v>3.2075999999999998</v>
+      </c>
+      <c r="C182">
+        <v>3.2154000000000002E-3</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A183" t="s">
+        <v>8</v>
+      </c>
+      <c r="B183">
+        <v>1.6906000000000001</v>
+      </c>
+      <c r="C183">
+        <v>1.1235999999999999E-2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A184" t="s">
+        <v>8</v>
+      </c>
+      <c r="B184">
+        <v>5.6337999999999999</v>
+      </c>
+      <c r="C184">
+        <v>4.6083000000000001E-3</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A185" t="s">
+        <v>8</v>
+      </c>
+      <c r="B185">
+        <v>3.202</v>
+      </c>
+      <c r="C185">
+        <v>8.0645000000000005E-3</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A186" t="s">
+        <v>8</v>
+      </c>
+      <c r="B186">
+        <v>0.70596999999999999</v>
+      </c>
+      <c r="C186">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A187" t="s">
+        <v>8</v>
+      </c>
+      <c r="B187">
+        <v>1.9032</v>
+      </c>
+      <c r="C187">
+        <v>1.6393000000000001E-2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A188" t="s">
+        <v>8</v>
+      </c>
+      <c r="B188">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C188">
+        <v>5.8479999999999999E-3</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A189" t="s">
+        <v>8</v>
+      </c>
+      <c r="B189">
+        <v>2.89</v>
+      </c>
+      <c r="C189">
+        <v>1.1494000000000001E-2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A190" t="s">
+        <v>8</v>
+      </c>
+      <c r="B190">
+        <v>0.52346999999999999</v>
+      </c>
+      <c r="C190">
+        <v>6.6667000000000002E-3</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A191" t="s">
+        <v>8</v>
+      </c>
+      <c r="B191">
+        <v>2.2473999999999998</v>
+      </c>
+      <c r="C191">
+        <v>1.0869999999999999E-2</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A192" t="s">
+        <v>8</v>
+      </c>
+      <c r="B192">
+        <v>2.8673000000000002</v>
+      </c>
+      <c r="C192">
+        <v>1.1235999999999999E-2</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A193" t="s">
+        <v>8</v>
+      </c>
+      <c r="B193">
+        <v>2.1608000000000001</v>
+      </c>
+      <c r="C193">
+        <v>1.2658000000000001E-2</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A194" t="s">
+        <v>8</v>
+      </c>
+      <c r="B194">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="C194">
+        <v>1.0101000000000001E-2</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A195" t="s">
+        <v>8</v>
+      </c>
+      <c r="B195">
+        <v>2.4</v>
+      </c>
+      <c r="C195">
+        <v>5.2082999999999999E-3</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A196" t="s">
+        <v>8</v>
+      </c>
+      <c r="B196">
+        <v>1.0458000000000001</v>
+      </c>
+      <c r="C196">
+        <v>1.0753E-2</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A197" t="s">
+        <v>8</v>
+      </c>
+      <c r="B197">
+        <v>2.3275000000000001</v>
+      </c>
+      <c r="C197">
+        <v>2.6667000000000001E-3</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A198" t="s">
+        <v>8</v>
+      </c>
+      <c r="B198">
+        <v>2.6758999999999999</v>
+      </c>
+      <c r="C198">
+        <v>1.0526000000000001E-2</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A199" t="s">
+        <v>8</v>
+      </c>
+      <c r="B199">
+        <v>5.4631999999999996</v>
+      </c>
+      <c r="C199">
+        <v>3.1846999999999999E-3</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A200" t="s">
+        <v>8</v>
+      </c>
+      <c r="B200">
+        <v>3.0333000000000001</v>
+      </c>
+      <c r="C200">
+        <v>9.7087000000000007E-3</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A201" t="s">
+        <v>8</v>
+      </c>
+      <c r="B201">
+        <v>2.1619999999999999</v>
+      </c>
+      <c r="C201">
+        <v>1.2987E-2</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A202" t="s">
+        <v>8</v>
+      </c>
+      <c r="B202">
+        <v>2.4138000000000002</v>
+      </c>
+      <c r="C202">
+        <v>8.5470000000000008E-3</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A203" t="s">
+        <v>8</v>
+      </c>
+      <c r="B203">
+        <v>1.1694</v>
+      </c>
+      <c r="C203">
+        <v>1.0309E-2</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A204" t="s">
+        <v>8</v>
+      </c>
+      <c r="B204">
+        <v>1.552</v>
+      </c>
+      <c r="C204">
+        <v>8.6957000000000007E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
debugging code on real txt files
</commit_message>
<xml_diff>
--- a/ptxdiffconc.xlsx
+++ b/ptxdiffconc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Feroze\Google Drive\DUKE 2016-2020\AxoSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7873B007-1032-42C0-85A9-1044C6E4E6C2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB1020F-B585-49E9-A88E-676CBA18013F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="7932" xr2:uid="{7C8E119D-E43A-48DC-A79E-D87DB8623B38}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="26">
   <si>
     <t>Amplitude</t>
   </si>
@@ -58,18 +58,74 @@
   <si>
     <t>ptx 200nM</t>
   </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>1.1.1</t>
+  </si>
+  <si>
+    <t>1.1.2</t>
+  </si>
+  <si>
+    <t>1.1.3</t>
+  </si>
+  <si>
+    <t>1.1.4</t>
+  </si>
+  <si>
+    <t>1.2.1</t>
+  </si>
+  <si>
+    <t>1.2.2</t>
+  </si>
+  <si>
+    <t>1.2.3</t>
+  </si>
+  <si>
+    <t>1.2.4</t>
+  </si>
+  <si>
+    <t>2.1.1</t>
+  </si>
+  <si>
+    <t>2.1.2</t>
+  </si>
+  <si>
+    <t>2.1.3</t>
+  </si>
+  <si>
+    <t>2.1.4</t>
+  </si>
+  <si>
+    <t>2.2.1</t>
+  </si>
+  <si>
+    <t>2.2.2</t>
+  </si>
+  <si>
+    <t>2.2.3</t>
+  </si>
+  <si>
+    <t>2.2.4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -92,8 +148,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,15 +468,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69CF060E-16C0-45EF-9C8D-C01CC13BD142}">
-  <dimension ref="A1:C204"/>
+  <dimension ref="A1:I204"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C204"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="11.47265625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -427,183 +490,423 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2">
-        <v>0.78193999999999997</v>
+        <v>1.3150999999999999</v>
       </c>
       <c r="C2">
-        <v>5.9172000000000001E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>4.9261000000000001E-3</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E2">
+        <f>D2-B2</f>
+        <v>1.1849000000000001</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <f>AVERAGE(B2:B17)</f>
+        <v>3.1864375000000003</v>
+      </c>
+      <c r="I2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B3">
-        <v>4.7279999999999998</v>
+        <v>3.8961999999999999</v>
       </c>
       <c r="C3">
-        <v>8.7718999999999991E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>8.1300999999999995E-3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E17" si="0">D3-B3</f>
+        <v>0.60380000000000011</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>1.0212000000000001</v>
+        <v>0.95199999999999996</v>
       </c>
       <c r="C4">
-        <v>5.3476000000000001E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>6.6667000000000002E-3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>4.548</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>2.3649</v>
+        <v>1.9466000000000001</v>
       </c>
       <c r="C5">
-        <v>9.1742999999999998E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>1.7857000000000001E-2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>5.3399999999999892E-2</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>2.4500000000000002</v>
+        <v>3.5076999999999998</v>
       </c>
       <c r="C6">
-        <v>4.0816000000000003E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>1.0309E-2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>-7.6999999999998181E-3</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>1.869</v>
+        <v>6.1231999999999998</v>
       </c>
       <c r="C7">
-        <v>1.0753E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>1.7240999999999999E-2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>-0.62319999999999975</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>5.3819999999999997</v>
+        <v>1.3118000000000001</v>
       </c>
       <c r="C8">
-        <v>6.4516E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>4.2193999999999999E-3</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>1.6881999999999999</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B9">
-        <v>8.0268999999999995</v>
+        <v>5.6630000000000003</v>
       </c>
       <c r="C9">
         <v>1.5873000000000002E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D9" s="1">
+        <v>6</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0.33699999999999974</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B10">
-        <v>3.6932</v>
+        <v>0.89817999999999998</v>
       </c>
       <c r="C10">
-        <v>6.6224999999999999E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>8.6957000000000007E-3</v>
+      </c>
+      <c r="D10" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>8.60182</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B11">
-        <v>1.4067000000000001</v>
+        <v>3.9590000000000001</v>
       </c>
       <c r="C11">
-        <v>1.5384999999999999E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>1.1110999999999999E-2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>-0.45900000000000007</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B12">
-        <v>0.74422999999999995</v>
+        <v>1.7578</v>
       </c>
       <c r="C12">
-        <v>7.3528999999999999E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>6.4516E-3</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0.24219999999999997</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B13">
-        <v>2.1949000000000001</v>
+        <v>6.8181000000000003</v>
       </c>
       <c r="C13">
-        <v>1.2987E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>1.2194999999999999E-2</v>
+      </c>
+      <c r="D13" s="1">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>-1.8181000000000003</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B14">
-        <v>1.18</v>
+        <v>2.4279000000000002</v>
       </c>
       <c r="C14">
-        <v>5.6179999999999997E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>3.4965E-3</v>
+      </c>
+      <c r="D14" s="1">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>1.5720999999999998</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B15">
-        <v>4.7469000000000001</v>
+        <v>4.7145000000000001</v>
       </c>
       <c r="C15">
-        <v>1.0869999999999999E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>1.0526000000000001E-2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0.78549999999999986</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B16">
-        <v>0.95365999999999995</v>
+        <v>0.60192000000000001</v>
       </c>
       <c r="C16">
-        <v>5.1282000000000003E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>9.1742999999999998E-3</v>
+      </c>
+      <c r="D16" s="1">
+        <v>13</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>12.39808</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B17">
-        <v>4.2706</v>
+        <v>5.09</v>
       </c>
       <c r="C17">
-        <v>1.3889E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="D17" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>1.4100000000000001</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I17">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -614,7 +917,7 @@
         <v>6.8027000000000001E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -625,7 +928,7 @@
         <v>1.7544000000000001E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -636,7 +939,7 @@
         <v>6.9443999999999999E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -647,7 +950,7 @@
         <v>1.0309E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -658,7 +961,7 @@
         <v>5.0251000000000002E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -669,7 +972,7 @@
         <v>1.7857000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -680,7 +983,7 @@
         <v>4.5455000000000001E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -691,7 +994,7 @@
         <v>1.2658000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -702,7 +1005,7 @@
         <v>1.1235999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -713,7 +1016,7 @@
         <v>1.0204E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -724,7 +1027,7 @@
         <v>9.8039000000000008E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -735,7 +1038,7 @@
         <v>1.2987E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -746,7 +1049,7 @@
         <v>4.5249000000000001E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -757,7 +1060,7 @@
         <v>1.1905000000000001E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
updating test files for axon segmentation
</commit_message>
<xml_diff>
--- a/ptxdiffconc.xlsx
+++ b/ptxdiffconc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Feroze\Google Drive\DUKE 2016-2020\AxoSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB1020F-B585-49E9-A88E-676CBA18013F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DFA7D0A-FA72-43FC-AD39-FF57BFE787F3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="7932" xr2:uid="{7C8E119D-E43A-48DC-A79E-D87DB8623B38}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="28">
   <si>
     <t>Amplitude</t>
   </si>
@@ -109,12 +109,21 @@
   <si>
     <t>2.2.4</t>
   </si>
+  <si>
+    <t>my ncv</t>
+  </si>
+  <si>
+    <t>hieu ncv</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,6 +133,18 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF4A86E8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -145,18 +166,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{5A514DEE-6B61-48C8-A9CB-724D5ABD1263}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -468,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69CF060E-16C0-45EF-9C8D-C01CC13BD142}">
-  <dimension ref="A1:I204"/>
+  <dimension ref="A1:R204"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="F77" sqref="F77:F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -479,7 +506,7 @@
     <col min="1" max="1" width="11.47265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -489,8 +516,14 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -518,8 +551,33 @@
       <c r="I2">
         <v>103</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="K2">
+        <v>4.9261000000000001E-3</v>
+      </c>
+      <c r="L2">
+        <f>1/K2</f>
+        <v>203.00034510058666</v>
+      </c>
+      <c r="M2">
+        <f>L2*0.05</f>
+        <v>10.150017255029333</v>
+      </c>
+      <c r="N2">
+        <v>4.2177777777777781</v>
+      </c>
+      <c r="P2">
+        <f>N2/M2</f>
+        <v>0.41554390222222226</v>
+      </c>
+      <c r="Q2">
+        <v>0.41760176017601758</v>
+      </c>
+      <c r="R2">
+        <f>(Q2-P2)*100/P2</f>
+        <v>0.49522034682506949</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -543,8 +601,33 @@
       <c r="I3">
         <v>104</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="K3">
+        <v>8.1300999999999995E-3</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L17" si="1">1/K3</f>
+        <v>122.99971710065067</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M17" si="2">L3*0.05</f>
+        <v>6.1499858550325337</v>
+      </c>
+      <c r="N3">
+        <v>1.6511111111111112</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P17" si="3">N3/M3</f>
+        <v>0.26847396888888891</v>
+      </c>
+      <c r="Q3">
+        <v>0.27067395264116573</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3:R17" si="4">(Q3-P3)*100/P3</f>
+        <v>0.81944024643495394</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -570,8 +653,33 @@
       <c r="I4">
         <v>105</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="K4">
+        <v>6.6667000000000002E-3</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="1"/>
+        <v>149.99925000374998</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="2"/>
+        <v>7.4999625001874994</v>
+      </c>
+      <c r="N4">
+        <v>3.1622222222222223</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="3"/>
+        <v>0.42163173777777774</v>
+      </c>
+      <c r="Q4">
+        <v>0.22269170579029729</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="4"/>
+        <v>-47.183362674735932</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -595,8 +703,33 @@
       <c r="I5">
         <v>106</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="K5">
+        <v>1.7857000000000001E-2</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>56.000448003584026</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="2"/>
+        <v>2.8000224001792016</v>
+      </c>
+      <c r="N5">
+        <v>1.2644444444444445</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="3"/>
+        <v>0.45158368888888889</v>
+      </c>
+      <c r="Q5">
+        <v>0.4863247863247861</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="4"/>
+        <v>7.693169237661543</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -620,8 +753,33 @@
       <c r="I6">
         <v>107</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="K6">
+        <v>1.0309E-2</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>97.0026190707149</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="2"/>
+        <v>4.8501309535357455</v>
+      </c>
+      <c r="N6">
+        <v>3.6311111111111112</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="3"/>
+        <v>0.74866248888888887</v>
+      </c>
+      <c r="Q6">
+        <v>0.55863247863247867</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="4"/>
+        <v>-25.382600714834677</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -645,8 +803,33 @@
       <c r="I7">
         <v>108</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="K7">
+        <v>1.7240999999999999E-2</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="1"/>
+        <v>58.001276028072617</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="2"/>
+        <v>2.9000638014036308</v>
+      </c>
+      <c r="N7">
+        <v>1.2955555555555556</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="3"/>
+        <v>0.44673346666666669</v>
+      </c>
+      <c r="Q7">
+        <v>0.33219373219373233</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="4"/>
+        <v>-25.639389707599182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -672,8 +855,33 @@
       <c r="I8">
         <v>109</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="K8">
+        <v>4.2193999999999999E-3</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>237.0005214011471</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="2"/>
+        <v>11.850026070057355</v>
+      </c>
+      <c r="N8">
+        <v>4.3511111111111109</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="3"/>
+        <v>0.36718156444444439</v>
+      </c>
+      <c r="Q8">
+        <v>0.30858944050433407</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="4"/>
+        <v>-15.957261914486851</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -697,8 +905,33 @@
       <c r="I9">
         <v>110</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="K9">
+        <v>1.5873000000000002E-2</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="1"/>
+        <v>63.000063000062994</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="2"/>
+        <v>3.1500031500031498</v>
+      </c>
+      <c r="N9">
+        <v>1.3244444444444445</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="3"/>
+        <v>0.42045813333333337</v>
+      </c>
+      <c r="Q9">
+        <v>0.33111111111111113</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="4"/>
+        <v>-21.249921249921254</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -724,8 +957,33 @@
       <c r="I10">
         <v>111</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="K10">
+        <v>8.6957000000000007E-3</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="1"/>
+        <v>114.99936750347872</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="2"/>
+        <v>5.7499683751739363</v>
+      </c>
+      <c r="N10">
+        <v>3.4488888888888889</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="3"/>
+        <v>0.59981006222222222</v>
+      </c>
+      <c r="Q10">
+        <v>0.24812150279776182</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="4"/>
+        <v>-58.63332104191413</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -749,8 +1007,33 @@
       <c r="I11">
         <v>112</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="K11">
+        <v>1.1110999999999999E-2</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>90.000900009000091</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="2"/>
+        <v>4.5000450004500046</v>
+      </c>
+      <c r="N11">
+        <v>1.1044444444444443</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="3"/>
+        <v>0.24542964444444443</v>
+      </c>
+      <c r="Q11">
+        <v>0.26937669376693757</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="4"/>
+        <v>9.7571951329269062</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -774,8 +1057,33 @@
       <c r="I12">
         <v>113</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="K12">
+        <v>6.4516E-3</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="1"/>
+        <v>155.00031000062</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="2"/>
+        <v>7.7500155000310009</v>
+      </c>
+      <c r="N12">
+        <v>3.86</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="3"/>
+        <v>0.49806351999999993</v>
+      </c>
+      <c r="Q12">
+        <v>0.45952380952380961</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="4"/>
+        <v>-7.7379107139166345</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -801,8 +1109,33 @@
       <c r="I13">
         <v>114</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="K13">
+        <v>1.2194999999999999E-2</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="1"/>
+        <v>82.000820008200094</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="2"/>
+        <v>4.1000410004100045</v>
+      </c>
+      <c r="N13">
+        <v>1.2977777777777777</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="3"/>
+        <v>0.31652799999999992</v>
+      </c>
+      <c r="Q13">
+        <v>0.3932659932659936</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="4"/>
+        <v>24.24366667909117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -828,8 +1161,33 @@
       <c r="I14">
         <v>115</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="K14">
+        <v>3.4965E-3</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="1"/>
+        <v>286.000286000286</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="2"/>
+        <v>14.300014300014301</v>
+      </c>
+      <c r="N14">
+        <v>3.82</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="3"/>
+        <v>0.2671326</v>
+      </c>
+      <c r="Q14">
+        <v>0.27092198581560278</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="4"/>
+        <v>1.4185411348531725</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -853,8 +1211,33 @@
       <c r="I15">
         <v>116</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="K15">
+        <v>1.0526000000000001E-2</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="1"/>
+        <v>95.002850085502558</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="2"/>
+        <v>4.7501425042751277</v>
+      </c>
+      <c r="N15">
+        <v>1.3577777777777778</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="3"/>
+        <v>0.28583937777777779</v>
+      </c>
+      <c r="Q15">
+        <v>0.29516908212560378</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="4"/>
+        <v>3.2639674842418827</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -880,8 +1263,33 @@
       <c r="I16">
         <v>117</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="K16">
+        <v>9.1742999999999998E-3</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="1"/>
+        <v>109.00014170018422</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="2"/>
+        <v>5.4500070850092115</v>
+      </c>
+      <c r="N16">
+        <v>3.8355555555555556</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="3"/>
+        <v>0.7037707466666665</v>
+      </c>
+      <c r="Q16">
+        <v>0.27996755879967555</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="4"/>
+        <v>-60.218926386794074</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -905,8 +1313,33 @@
       <c r="I17">
         <v>118</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="K17">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="N17">
+        <v>1.3288888888888888</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="3"/>
+        <v>0.3322222222222222</v>
+      </c>
+      <c r="Q17">
+        <v>0.34074074074074084</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="4"/>
+        <v>2.564102564102603</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -916,8 +1349,16 @@
       <c r="C18">
         <v>6.8027000000000001E-3</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="P18">
+        <f>AVERAGE(P2:P17)</f>
+        <v>0.42431657027777769</v>
+      </c>
+      <c r="Q18">
+        <f>AVERAGE(Q2:Q17)</f>
+        <v>0.34280664588812804</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -928,7 +1369,7 @@
         <v>1.7544000000000001E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -939,7 +1380,7 @@
         <v>6.9443999999999999E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -950,7 +1391,7 @@
         <v>1.0309E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -961,7 +1402,7 @@
         <v>5.0251000000000002E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -972,7 +1413,7 @@
         <v>1.7857000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -983,7 +1424,7 @@
         <v>4.5455000000000001E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -994,7 +1435,7 @@
         <v>1.2658000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -1005,7 +1446,7 @@
         <v>1.1235999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -1016,7 +1457,7 @@
         <v>1.0204E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -1027,7 +1468,7 @@
         <v>9.8039000000000008E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -1038,7 +1479,7 @@
         <v>1.2987E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -1049,7 +1490,7 @@
         <v>4.5249000000000001E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -1060,7 +1501,7 @@
         <v>1.1905000000000001E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -1423,7 +1864,7 @@
         <v>1.1110999999999999E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
         <v>3</v>
       </c>
@@ -1434,7 +1875,7 @@
         <v>5.4348E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
         <v>3</v>
       </c>
@@ -1445,7 +1886,7 @@
         <v>8.6957000000000007E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
         <v>3</v>
       </c>
@@ -1456,7 +1897,7 @@
         <v>1.0989000000000001E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
         <v>3</v>
       </c>
@@ -1467,7 +1908,7 @@
         <v>1.9231000000000002E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
         <v>3</v>
       </c>
@@ -1478,7 +1919,7 @@
         <v>5.5249000000000001E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
         <v>3</v>
       </c>
@@ -1489,7 +1930,7 @@
         <v>1.7544000000000001E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
         <v>3</v>
       </c>
@@ -1500,7 +1941,7 @@
         <v>6.5789000000000004E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
         <v>3</v>
       </c>
@@ -1511,7 +1952,7 @@
         <v>7.7518999999999999E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
         <v>3</v>
       </c>
@@ -1522,7 +1963,7 @@
         <v>9.3457999999999996E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
         <v>3</v>
       </c>
@@ -1533,7 +1974,7 @@
         <v>1.0204E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
         <v>3</v>
       </c>
@@ -1544,7 +1985,7 @@
         <v>3.9683000000000001E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
         <v>3</v>
       </c>
@@ -1555,7 +1996,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
         <v>4</v>
       </c>
@@ -1565,8 +2006,16 @@
       <c r="C77">
         <v>7.5757999999999997E-3</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E77">
+        <f>0.05/C77</f>
+        <v>6.5999630402069753</v>
+      </c>
+      <c r="F77" s="4">
+        <f t="shared" ref="F77:F84" si="5">E77/450</f>
+        <v>1.4666584533793279E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
         <v>4</v>
       </c>
@@ -1576,8 +2025,16 @@
       <c r="C78">
         <v>4.5662000000000003E-3</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E78">
+        <f t="shared" ref="E78:E91" si="6">0.05/C78</f>
+        <v>10.950024090052999</v>
+      </c>
+      <c r="F78" s="4">
+        <f t="shared" si="5"/>
+        <v>2.4333386866784441E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
         <v>4</v>
       </c>
@@ -1587,8 +2044,16 @@
       <c r="C79">
         <v>5.2356E-3</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E79">
+        <f t="shared" si="6"/>
+        <v>9.5500038200015283</v>
+      </c>
+      <c r="F79" s="5">
+        <f t="shared" si="5"/>
+        <v>2.1222230711114506E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
         <v>4</v>
       </c>
@@ -1598,8 +2063,16 @@
       <c r="C80">
         <v>8.1300999999999995E-3</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E80">
+        <f t="shared" si="6"/>
+        <v>6.1499858550325346</v>
+      </c>
+      <c r="F80" s="5">
+        <f t="shared" si="5"/>
+        <v>1.3666635233405633E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
         <v>4</v>
       </c>
@@ -1609,8 +2082,16 @@
       <c r="C81">
         <v>3.3557000000000001E-3</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E81">
+        <f t="shared" si="6"/>
+        <v>14.900020860029205</v>
+      </c>
+      <c r="F81" s="4">
+        <f t="shared" si="5"/>
+        <v>3.3111157466731565E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
         <v>4</v>
       </c>
@@ -1620,8 +2101,16 @@
       <c r="C82">
         <v>9.4339999999999997E-3</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E82">
+        <f t="shared" si="6"/>
+        <v>5.2999788000848005</v>
+      </c>
+      <c r="F82" s="4">
+        <f t="shared" si="5"/>
+        <v>1.1777730666855113E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" t="s">
         <v>4</v>
       </c>
@@ -1631,8 +2120,13 @@
       <c r="C83">
         <v>3.3333E-3</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E83">
+        <f t="shared" si="6"/>
+        <v>15.000150001500016</v>
+      </c>
+      <c r="F83" s="4"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
         <v>4</v>
       </c>
@@ -1642,8 +2136,13 @@
       <c r="C84">
         <v>8.6957000000000007E-3</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E84">
+        <f t="shared" si="6"/>
+        <v>5.7499683751739363</v>
+      </c>
+      <c r="F84" s="4"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
         <v>4</v>
       </c>
@@ -1653,8 +2152,13 @@
       <c r="C85">
         <v>6.2112000000000001E-3</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E85">
+        <f t="shared" si="6"/>
+        <v>8.0499742400824328</v>
+      </c>
+      <c r="F85" s="3"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
         <v>4</v>
       </c>
@@ -1664,8 +2168,13 @@
       <c r="C86">
         <v>6.1728E-3</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E86">
+        <f t="shared" si="6"/>
+        <v>8.1000518403317781</v>
+      </c>
+      <c r="F86" s="3"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
         <v>4</v>
       </c>
@@ -1675,8 +2184,13 @@
       <c r="C87">
         <v>9.0909000000000007E-3</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E87">
+        <f t="shared" si="6"/>
+        <v>5.5000055000054999</v>
+      </c>
+      <c r="F87" s="3"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="s">
         <v>4</v>
       </c>
@@ -1686,8 +2200,13 @@
       <c r="C88">
         <v>6.7568000000000003E-3</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E88">
+        <f t="shared" si="6"/>
+        <v>7.399952640303102</v>
+      </c>
+      <c r="F88" s="3"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" t="s">
         <v>4</v>
       </c>
@@ -1697,8 +2216,13 @@
       <c r="C89">
         <v>3.0303000000000001E-3</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E89">
+        <f t="shared" si="6"/>
+        <v>16.5000165000165</v>
+      </c>
+      <c r="F89" s="6"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
         <v>4</v>
       </c>
@@ -1708,8 +2232,13 @@
       <c r="C90">
         <v>8.4034000000000001E-3</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E90">
+        <f t="shared" si="6"/>
+        <v>5.9499726301259015</v>
+      </c>
+      <c r="F90" s="6"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" t="s">
         <v>4</v>
       </c>
@@ -1719,8 +2248,19 @@
       <c r="C91">
         <v>8.3333000000000001E-3</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E91">
+        <f t="shared" si="6"/>
+        <v>6.0000240000960003</v>
+      </c>
+      <c r="F91" s="6"/>
+      <c r="I91" t="s">
+        <v>26</v>
+      </c>
+      <c r="J91" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="s">
         <v>5</v>
       </c>
@@ -1730,8 +2270,22 @@
       <c r="C92">
         <v>5.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="F92" s="6">
+        <f>0.05/C92</f>
+        <v>10</v>
+      </c>
+      <c r="G92">
+        <v>3.2488888888888887</v>
+      </c>
+      <c r="I92">
+        <f>G92/F92</f>
+        <v>0.32488888888888889</v>
+      </c>
+      <c r="J92">
+        <v>0.36504369538077408</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
         <v>5</v>
       </c>
@@ -1741,8 +2295,22 @@
       <c r="C93">
         <v>7.5757999999999997E-3</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="F93" s="6">
+        <f t="shared" ref="F93:F103" si="7">0.05/C93</f>
+        <v>6.5999630402069753</v>
+      </c>
+      <c r="G93">
+        <v>4.96</v>
+      </c>
+      <c r="I93">
+        <f t="shared" ref="I93:I103" si="8">G93/F93</f>
+        <v>0.75151935999999997</v>
+      </c>
+      <c r="J93">
+        <v>0.2740331491712707</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
         <v>5</v>
       </c>
@@ -1752,8 +2320,22 @@
       <c r="C94">
         <v>5.0761000000000001E-3</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="F94" s="6">
+        <f t="shared" si="7"/>
+        <v>9.8500817556785734</v>
+      </c>
+      <c r="G94">
+        <v>5.5111111111111111</v>
+      </c>
+      <c r="I94">
+        <f t="shared" si="8"/>
+        <v>0.55949902222222214</v>
+      </c>
+      <c r="J94">
+        <v>0.42393162393162392</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
         <v>5</v>
       </c>
@@ -1763,8 +2345,22 @@
       <c r="C95">
         <v>7.7518999999999999E-3</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="F95" s="6">
+        <f t="shared" si="7"/>
+        <v>6.4500316051548658</v>
+      </c>
+      <c r="G95">
+        <v>5.2044444444444444</v>
+      </c>
+      <c r="I95">
+        <f t="shared" si="8"/>
+        <v>0.80688665777777768</v>
+      </c>
+      <c r="J95">
+        <v>0.49566137566137564</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
         <v>5</v>
       </c>
@@ -1774,8 +2370,22 @@
       <c r="C96">
         <v>7.9365000000000008E-3</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="F96" s="6">
+        <f t="shared" si="7"/>
+        <v>6.3000063000062996</v>
+      </c>
+      <c r="G96">
+        <v>4.0333333333333332</v>
+      </c>
+      <c r="I96">
+        <f t="shared" si="8"/>
+        <v>0.64021099999999997</v>
+      </c>
+      <c r="J96">
+        <v>0.39158576051779947</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
         <v>5</v>
       </c>
@@ -1785,8 +2395,22 @@
       <c r="C97">
         <v>8.6957000000000007E-3</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="F97" s="6">
+        <f t="shared" si="7"/>
+        <v>5.7499683751739363</v>
+      </c>
+      <c r="G97">
+        <v>4.1288888888888886</v>
+      </c>
+      <c r="I97">
+        <f t="shared" si="8"/>
+        <v>0.71807158222222223</v>
+      </c>
+      <c r="J97">
+        <v>0.38951781970649885</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
         <v>5</v>
       </c>
@@ -1796,8 +2420,22 @@
       <c r="C98">
         <v>6.6224999999999999E-3</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="F98" s="6">
+        <f t="shared" si="7"/>
+        <v>7.5500188750471882</v>
+      </c>
+      <c r="G98">
+        <v>4.1933333333333334</v>
+      </c>
+      <c r="I98">
+        <f t="shared" si="8"/>
+        <v>0.55540699999999998</v>
+      </c>
+      <c r="J98">
+        <v>0.43230240549828164</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
         <v>5</v>
       </c>
@@ -1807,8 +2445,22 @@
       <c r="C99">
         <v>1.2194999999999999E-2</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="F99" s="6">
+        <f t="shared" si="7"/>
+        <v>4.1000410004100045</v>
+      </c>
+      <c r="G99">
+        <v>4.1266666666666669</v>
+      </c>
+      <c r="I99">
+        <f t="shared" si="8"/>
+        <v>1.006494</v>
+      </c>
+      <c r="J99">
+        <v>0.44855072463768103</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
         <v>5</v>
       </c>
@@ -1818,8 +2470,22 @@
       <c r="C100">
         <v>3.9215999999999999E-3</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="F100" s="6">
+        <f t="shared" si="7"/>
+        <v>12.749898000815994</v>
+      </c>
+      <c r="G100">
+        <v>4.3133333333333335</v>
+      </c>
+      <c r="I100">
+        <f t="shared" si="8"/>
+        <v>0.33830336</v>
+      </c>
+      <c r="J100">
+        <v>0.26958333333333334</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
         <v>5</v>
       </c>
@@ -1829,8 +2495,22 @@
       <c r="C101">
         <v>1.1627999999999999E-2</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="F101" s="6">
+        <f t="shared" si="7"/>
+        <v>4.2999656002751978</v>
+      </c>
+      <c r="G101">
+        <v>1.5733333333333333</v>
+      </c>
+      <c r="I101">
+        <f t="shared" si="8"/>
+        <v>0.36589439999999995</v>
+      </c>
+      <c r="J101">
+        <v>0.43703703703703684</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
         <v>5</v>
       </c>
@@ -1840,8 +2520,22 @@
       <c r="C102">
         <v>3.5971000000000002E-3</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="F102" s="6">
+        <f t="shared" si="7"/>
+        <v>13.90008618053432</v>
+      </c>
+      <c r="G102">
+        <v>5.0177777777777779</v>
+      </c>
+      <c r="I102">
+        <f t="shared" si="8"/>
+        <v>0.36098896888888887</v>
+      </c>
+      <c r="J102">
+        <v>0.36895424836601304</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
         <v>5</v>
       </c>
@@ -1851,8 +2545,22 @@
       <c r="C103">
         <v>1.1627999999999999E-2</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="F103" s="6">
+        <f t="shared" si="7"/>
+        <v>4.2999656002751978</v>
+      </c>
+      <c r="G103">
+        <v>1.6311111111111112</v>
+      </c>
+      <c r="I103">
+        <f t="shared" si="8"/>
+        <v>0.37933120000000004</v>
+      </c>
+      <c r="J103">
+        <v>0.38835978835978813</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
         <v>6</v>
       </c>
@@ -1862,8 +2570,16 @@
       <c r="C104">
         <v>4.9261000000000001E-3</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="I104">
+        <f>AVERAGE(I92:I103)</f>
+        <v>0.56729128666666673</v>
+      </c>
+      <c r="J104">
+        <f>AVERAGE(J92:J103)</f>
+        <v>0.39038008013345643</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
         <v>6</v>
       </c>
@@ -1874,7 +2590,7 @@
         <v>8.1300999999999995E-3</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
         <v>6</v>
       </c>
@@ -1885,7 +2601,7 @@
         <v>6.6667000000000002E-3</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
         <v>6</v>
       </c>
@@ -1896,7 +2612,7 @@
         <v>1.7857000000000001E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
         <v>6</v>
       </c>
@@ -1907,7 +2623,7 @@
         <v>1.0309E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
         <v>6</v>
       </c>
@@ -1918,7 +2634,7 @@
         <v>1.7240999999999999E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
         <v>6</v>
       </c>
@@ -1929,7 +2645,7 @@
         <v>4.2193999999999999E-3</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" t="s">
         <v>6</v>
       </c>
@@ -1940,7 +2656,7 @@
         <v>1.5873000000000002E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
using the median of all traces rather than just the mean trace leads to robustness in the model
</commit_message>
<xml_diff>
--- a/ptxdiffconc.xlsx
+++ b/ptxdiffconc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Feroze\Google Drive\DUKE 2016-2020\AxoSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DFA7D0A-FA72-43FC-AD39-FF57BFE787F3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{379BCEA2-792E-4A20-B849-FE0D1E2F9D1F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="7932" xr2:uid="{7C8E119D-E43A-48DC-A79E-D87DB8623B38}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="31">
   <si>
     <t>Amplitude</t>
   </si>
@@ -115,6 +115,15 @@
   <si>
     <t>hieu ncv</t>
   </si>
+  <si>
+    <t>stdev</t>
+  </si>
+  <si>
+    <t>% difference</t>
+  </si>
+  <si>
+    <t>latency</t>
+  </si>
 </sst>
 </file>
 
@@ -123,7 +132,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,6 +157,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -170,7 +187,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -180,6 +197,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,18 +513,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69CF060E-16C0-45EF-9C8D-C01CC13BD142}">
-  <dimension ref="A1:R204"/>
+  <dimension ref="A1:S204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="F77" sqref="F77:F84"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.47265625" customWidth="1"/>
+    <col min="1" max="1" width="16.5234375" customWidth="1"/>
+    <col min="18" max="18" width="11.3671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -516,14 +535,23 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="L1" t="s">
+        <v>30</v>
+      </c>
       <c r="P1" t="s">
         <v>26</v>
       </c>
       <c r="Q1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="R1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -555,29 +583,31 @@
         <v>4.9261000000000001E-3</v>
       </c>
       <c r="L2">
-        <f>1/K2</f>
-        <v>203.00034510058666</v>
+        <v>250</v>
       </c>
       <c r="M2">
         <f>L2*0.05</f>
-        <v>10.150017255029333</v>
+        <v>12.5</v>
       </c>
       <c r="N2">
         <v>4.2177777777777781</v>
       </c>
       <c r="P2">
         <f>N2/M2</f>
-        <v>0.41554390222222226</v>
+        <v>0.33742222222222223</v>
       </c>
       <c r="Q2">
         <v>0.41760176017601758</v>
       </c>
       <c r="R2">
         <f>(Q2-P2)*100/P2</f>
-        <v>0.49522034682506949</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>23.762376237623752</v>
+      </c>
+      <c r="S2">
+        <v>56.974800000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -605,29 +635,31 @@
         <v>8.1300999999999995E-3</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L17" si="1">1/K3</f>
-        <v>122.99971710065067</v>
+        <v>128.5</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M17" si="2">L3*0.05</f>
-        <v>6.1499858550325337</v>
+        <f t="shared" ref="M3:M17" si="1">L3*0.05</f>
+        <v>6.4250000000000007</v>
       </c>
       <c r="N3">
         <v>1.6511111111111112</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P17" si="3">N3/M3</f>
-        <v>0.26847396888888891</v>
+        <f t="shared" ref="P3:P17" si="2">N3/M3</f>
+        <v>0.25698227410289665</v>
       </c>
       <c r="Q3">
         <v>0.27067395264116573</v>
       </c>
       <c r="R3">
-        <f t="shared" ref="R3:R17" si="4">(Q3-P3)*100/P3</f>
-        <v>0.81944024643495394</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" ref="R3:R17" si="3">(Q3-P3)*100/P3</f>
+        <v>5.327868852459015</v>
+      </c>
+      <c r="S3">
+        <v>22.8279</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -657,29 +689,31 @@
         <v>6.6667000000000002E-3</v>
       </c>
       <c r="L4">
+        <v>281</v>
+      </c>
+      <c r="M4">
         <f t="shared" si="1"/>
-        <v>149.99925000374998</v>
-      </c>
-      <c r="M4">
-        <f t="shared" si="2"/>
-        <v>7.4999625001874994</v>
+        <v>14.05</v>
       </c>
       <c r="N4">
         <v>3.1622222222222223</v>
       </c>
       <c r="P4">
-        <f t="shared" si="3"/>
-        <v>0.42163173777777774</v>
+        <f t="shared" si="2"/>
+        <v>0.22506919731119018</v>
       </c>
       <c r="Q4">
         <v>0.22269170579029729</v>
       </c>
       <c r="R4">
-        <f t="shared" si="4"/>
-        <v>-47.183362674735932</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="3"/>
+        <v>-1.0563380281690318</v>
+      </c>
+      <c r="S4">
+        <v>13.6158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -707,29 +741,31 @@
         <v>1.7857000000000001E-2</v>
       </c>
       <c r="L5">
+        <v>139</v>
+      </c>
+      <c r="M5">
         <f t="shared" si="1"/>
-        <v>56.000448003584026</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="2"/>
-        <v>2.8000224001792016</v>
+        <v>6.95</v>
       </c>
       <c r="N5">
         <v>1.2644444444444445</v>
       </c>
       <c r="P5">
-        <f t="shared" si="3"/>
-        <v>0.45158368888888889</v>
+        <f t="shared" si="2"/>
+        <v>0.18193445243804957</v>
       </c>
       <c r="Q5">
         <v>0.4863247863247861</v>
       </c>
-      <c r="R5">
-        <f t="shared" si="4"/>
-        <v>7.693169237661543</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="R5" s="7">
+        <f t="shared" si="3"/>
+        <v>167.30769230769218</v>
+      </c>
+      <c r="S5">
+        <v>105.62479999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -757,29 +793,31 @@
         <v>1.0309E-2</v>
       </c>
       <c r="L6">
+        <v>333</v>
+      </c>
+      <c r="M6">
         <f t="shared" si="1"/>
-        <v>97.0026190707149</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="2"/>
-        <v>4.8501309535357455</v>
+        <v>16.650000000000002</v>
       </c>
       <c r="N6">
         <v>3.6311111111111112</v>
       </c>
       <c r="P6">
-        <f t="shared" si="3"/>
-        <v>0.74866248888888887</v>
+        <f t="shared" si="2"/>
+        <v>0.21808475141808473</v>
       </c>
       <c r="Q6">
         <v>0.55863247863247867</v>
       </c>
-      <c r="R6">
-        <f t="shared" si="4"/>
-        <v>-25.382600714834677</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="R6" s="7">
+        <f t="shared" si="3"/>
+        <v>156.15384615384622</v>
+      </c>
+      <c r="S6">
+        <v>161.63900000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -807,29 +845,31 @@
         <v>1.7240999999999999E-2</v>
       </c>
       <c r="L7">
+        <v>83</v>
+      </c>
+      <c r="M7">
         <f t="shared" si="1"/>
-        <v>58.001276028072617</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="2"/>
-        <v>2.9000638014036308</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="N7">
         <v>1.2955555555555556</v>
       </c>
       <c r="P7">
-        <f t="shared" si="3"/>
-        <v>0.44673346666666669</v>
+        <f t="shared" si="2"/>
+        <v>0.31218206157965189</v>
       </c>
       <c r="Q7">
         <v>0.33219373219373233</v>
       </c>
       <c r="R7">
-        <f t="shared" si="4"/>
-        <v>-25.639389707599182</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="3"/>
+        <v>6.4102564102564701</v>
+      </c>
+      <c r="S7">
+        <v>160.29040000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -859,29 +899,31 @@
         <v>4.2193999999999999E-3</v>
       </c>
       <c r="L8">
+        <v>300.5</v>
+      </c>
+      <c r="M8">
         <f t="shared" si="1"/>
-        <v>237.0005214011471</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="2"/>
-        <v>11.850026070057355</v>
+        <v>15.025</v>
       </c>
       <c r="N8">
         <v>4.3511111111111109</v>
       </c>
       <c r="P8">
-        <f t="shared" si="3"/>
-        <v>0.36718156444444439</v>
+        <f t="shared" si="2"/>
+        <v>0.28959142170456642</v>
       </c>
       <c r="Q8">
         <v>0.30858944050433407</v>
       </c>
       <c r="R8">
-        <f t="shared" si="4"/>
-        <v>-15.957261914486851</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="3"/>
+        <v>6.5602836879432598</v>
+      </c>
+      <c r="S8">
+        <v>222.41390000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -909,29 +951,31 @@
         <v>1.5873000000000002E-2</v>
       </c>
       <c r="L9">
+        <v>83</v>
+      </c>
+      <c r="M9">
         <f t="shared" si="1"/>
-        <v>63.000063000062994</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="2"/>
-        <v>3.1500031500031498</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="N9">
         <v>1.3244444444444445</v>
       </c>
       <c r="P9">
-        <f t="shared" si="3"/>
-        <v>0.42045813333333337</v>
+        <f t="shared" si="2"/>
+        <v>0.31914323962516733</v>
       </c>
       <c r="Q9">
         <v>0.33111111111111113</v>
       </c>
       <c r="R9">
-        <f t="shared" si="4"/>
-        <v>-21.249921249921254</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="3"/>
+        <v>3.7500000000000093</v>
+      </c>
+      <c r="S9">
+        <v>67.884799999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -961,29 +1005,31 @@
         <v>8.6957000000000007E-3</v>
       </c>
       <c r="L10">
+        <v>280</v>
+      </c>
+      <c r="M10">
         <f t="shared" si="1"/>
-        <v>114.99936750347872</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="2"/>
-        <v>5.7499683751739363</v>
+        <v>14</v>
       </c>
       <c r="N10">
         <v>3.4488888888888889</v>
       </c>
       <c r="P10">
-        <f t="shared" si="3"/>
-        <v>0.59981006222222222</v>
+        <f t="shared" si="2"/>
+        <v>0.24634920634920635</v>
       </c>
       <c r="Q10">
         <v>0.24812150279776182</v>
       </c>
       <c r="R10">
-        <f t="shared" si="4"/>
-        <v>-58.63332104191413</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="3"/>
+        <v>0.71942446043166919</v>
+      </c>
+      <c r="S10">
+        <v>79.450400000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1011,29 +1057,31 @@
         <v>1.1110999999999999E-2</v>
       </c>
       <c r="L11">
+        <v>141</v>
+      </c>
+      <c r="M11">
         <f t="shared" si="1"/>
-        <v>90.000900009000091</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="2"/>
-        <v>4.5000450004500046</v>
+        <v>7.0500000000000007</v>
       </c>
       <c r="N11">
         <v>1.1044444444444443</v>
       </c>
       <c r="P11">
-        <f t="shared" si="3"/>
-        <v>0.24542964444444443</v>
+        <f t="shared" si="2"/>
+        <v>0.15665878644602046</v>
       </c>
       <c r="Q11">
         <v>0.26937669376693757</v>
       </c>
-      <c r="R11">
-        <f t="shared" si="4"/>
-        <v>9.7571951329269062</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="R11" s="7">
+        <f t="shared" si="3"/>
+        <v>71.951219512195081</v>
+      </c>
+      <c r="S11">
+        <v>116.1221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1061,29 +1109,31 @@
         <v>6.4516E-3</v>
       </c>
       <c r="L12">
+        <v>196</v>
+      </c>
+      <c r="M12">
         <f t="shared" si="1"/>
-        <v>155.00031000062</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="2"/>
-        <v>7.7500155000310009</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="N12">
         <v>3.86</v>
       </c>
       <c r="P12">
-        <f t="shared" si="3"/>
-        <v>0.49806351999999993</v>
+        <f t="shared" si="2"/>
+        <v>0.39387755102040811</v>
       </c>
       <c r="Q12">
         <v>0.45952380952380961</v>
       </c>
       <c r="R12">
-        <f t="shared" si="4"/>
-        <v>-7.7379107139166345</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="3"/>
+        <v>16.666666666666703</v>
+      </c>
+      <c r="S12">
+        <v>133.98830000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1113,29 +1163,31 @@
         <v>1.2194999999999999E-2</v>
       </c>
       <c r="L13">
+        <v>82</v>
+      </c>
+      <c r="M13">
         <f t="shared" si="1"/>
-        <v>82.000820008200094</v>
-      </c>
-      <c r="M13">
-        <f t="shared" si="2"/>
-        <v>4.1000410004100045</v>
+        <v>4.1000000000000005</v>
       </c>
       <c r="N13">
         <v>1.2977777777777777</v>
       </c>
       <c r="P13">
-        <f t="shared" si="3"/>
-        <v>0.31652799999999992</v>
+        <f t="shared" si="2"/>
+        <v>0.31653116531165304</v>
       </c>
       <c r="Q13">
         <v>0.3932659932659936</v>
       </c>
       <c r="R13">
-        <f t="shared" si="4"/>
-        <v>24.24366667909117</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="3"/>
+        <v>24.242424242424377</v>
+      </c>
+      <c r="S13">
+        <v>101.732</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -1165,29 +1217,31 @@
         <v>3.4965E-3</v>
       </c>
       <c r="L14">
+        <v>297</v>
+      </c>
+      <c r="M14">
         <f t="shared" si="1"/>
-        <v>286.000286000286</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="2"/>
-        <v>14.300014300014301</v>
+        <v>14.850000000000001</v>
       </c>
       <c r="N14">
         <v>3.82</v>
       </c>
       <c r="P14">
-        <f t="shared" si="3"/>
-        <v>0.2671326</v>
+        <f t="shared" si="2"/>
+        <v>0.25723905723905721</v>
       </c>
       <c r="Q14">
         <v>0.27092198581560278</v>
       </c>
       <c r="R14">
-        <f t="shared" si="4"/>
-        <v>1.4185411348531725</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="3"/>
+        <v>5.3191489361702038</v>
+      </c>
+      <c r="S14">
+        <v>86.057599999999994</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1215,29 +1269,31 @@
         <v>1.0526000000000001E-2</v>
       </c>
       <c r="L15">
+        <v>94</v>
+      </c>
+      <c r="M15">
         <f t="shared" si="1"/>
-        <v>95.002850085502558</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="2"/>
-        <v>4.7501425042751277</v>
+        <v>4.7</v>
       </c>
       <c r="N15">
         <v>1.3577777777777778</v>
       </c>
       <c r="P15">
-        <f t="shared" si="3"/>
-        <v>0.28583937777777779</v>
+        <f t="shared" si="2"/>
+        <v>0.28888888888888886</v>
       </c>
       <c r="Q15">
         <v>0.29516908212560378</v>
       </c>
       <c r="R15">
-        <f t="shared" si="4"/>
-        <v>3.2639674842418827</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="3"/>
+        <v>2.1739130434782399</v>
+      </c>
+      <c r="S15">
+        <v>105.4444</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1267,29 +1323,31 @@
         <v>9.1742999999999998E-3</v>
       </c>
       <c r="L16">
+        <v>275</v>
+      </c>
+      <c r="M16">
         <f t="shared" si="1"/>
-        <v>109.00014170018422</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="2"/>
-        <v>5.4500070850092115</v>
+        <v>13.75</v>
       </c>
       <c r="N16">
         <v>3.8355555555555556</v>
       </c>
       <c r="P16">
-        <f t="shared" si="3"/>
-        <v>0.7037707466666665</v>
+        <f t="shared" si="2"/>
+        <v>0.27894949494949495</v>
       </c>
       <c r="Q16">
         <v>0.27996755879967555</v>
       </c>
       <c r="R16">
-        <f t="shared" si="4"/>
-        <v>-60.218926386794074</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="3"/>
+        <v>0.36496350364962343</v>
+      </c>
+      <c r="S16">
+        <v>153.54339999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1317,29 +1375,31 @@
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="L17">
+        <v>79</v>
+      </c>
+      <c r="M17">
         <f t="shared" si="1"/>
-        <v>80</v>
-      </c>
-      <c r="M17">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <v>3.95</v>
       </c>
       <c r="N17">
         <v>1.3288888888888888</v>
       </c>
       <c r="P17">
-        <f t="shared" si="3"/>
-        <v>0.3322222222222222</v>
+        <f t="shared" si="2"/>
+        <v>0.33642756680731362</v>
       </c>
       <c r="Q17">
         <v>0.34074074074074084</v>
       </c>
       <c r="R17">
-        <f t="shared" si="4"/>
-        <v>2.564102564102603</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" si="3"/>
+        <v>1.2820512820513208</v>
+      </c>
+      <c r="S17">
+        <v>83.590100000000007</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -1351,14 +1411,18 @@
       </c>
       <c r="P18">
         <f>AVERAGE(P2:P17)</f>
-        <v>0.42431657027777769</v>
+        <v>0.275958208588367</v>
       </c>
       <c r="Q18">
         <f>AVERAGE(Q2:Q17)</f>
         <v>0.34280664588812804</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="R18">
+        <f>AVERAGE(R2:R17)</f>
+        <v>30.683487329294941</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -1368,8 +1432,12 @@
       <c r="C19">
         <v>1.7544000000000001E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q19">
+        <f>(Q18-P18)*100/Q18</f>
+        <v>19.500332943246509</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -1380,7 +1448,7 @@
         <v>6.9443999999999999E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -1391,7 +1459,7 @@
         <v>1.0309E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -1402,7 +1470,7 @@
         <v>5.0251000000000002E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -1413,7 +1481,7 @@
         <v>1.7857000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -1424,7 +1492,7 @@
         <v>4.5455000000000001E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -1435,7 +1503,7 @@
         <v>1.2658000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -1446,7 +1514,7 @@
         <v>1.1235999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -1457,7 +1525,7 @@
         <v>1.0204E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -1468,7 +1536,7 @@
         <v>9.8039000000000008E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -1479,7 +1547,7 @@
         <v>1.2987E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -1490,7 +1558,7 @@
         <v>4.5249000000000001E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -1501,7 +1569,7 @@
         <v>1.1905000000000001E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -2011,7 +2079,7 @@
         <v>6.5999630402069753</v>
       </c>
       <c r="F77" s="4">
-        <f t="shared" ref="F77:F84" si="5">E77/450</f>
+        <f t="shared" ref="F77:F82" si="4">E77/450</f>
         <v>1.4666584533793279E-2</v>
       </c>
     </row>
@@ -2026,11 +2094,11 @@
         <v>4.5662000000000003E-3</v>
       </c>
       <c r="E78">
-        <f t="shared" ref="E78:E91" si="6">0.05/C78</f>
+        <f t="shared" ref="E78:E91" si="5">0.05/C78</f>
         <v>10.950024090052999</v>
       </c>
       <c r="F78" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.4333386866784441E-2</v>
       </c>
     </row>
@@ -2045,11 +2113,11 @@
         <v>5.2356E-3</v>
       </c>
       <c r="E79">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>9.5500038200015283</v>
       </c>
       <c r="F79" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.1222230711114506E-2</v>
       </c>
     </row>
@@ -2064,11 +2132,11 @@
         <v>8.1300999999999995E-3</v>
       </c>
       <c r="E80">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>6.1499858550325346</v>
       </c>
       <c r="F80" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.3666635233405633E-2</v>
       </c>
     </row>
@@ -2083,11 +2151,11 @@
         <v>3.3557000000000001E-3</v>
       </c>
       <c r="E81">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>14.900020860029205</v>
       </c>
       <c r="F81" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.3111157466731565E-2</v>
       </c>
     </row>
@@ -2102,11 +2170,11 @@
         <v>9.4339999999999997E-3</v>
       </c>
       <c r="E82">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>5.2999788000848005</v>
       </c>
       <c r="F82" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.1777730666855113E-2</v>
       </c>
     </row>
@@ -2121,7 +2189,7 @@
         <v>3.3333E-3</v>
       </c>
       <c r="E83">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>15.000150001500016</v>
       </c>
       <c r="F83" s="4"/>
@@ -2137,7 +2205,7 @@
         <v>8.6957000000000007E-3</v>
       </c>
       <c r="E84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>5.7499683751739363</v>
       </c>
       <c r="F84" s="4"/>
@@ -2153,7 +2221,7 @@
         <v>6.2112000000000001E-3</v>
       </c>
       <c r="E85">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>8.0499742400824328</v>
       </c>
       <c r="F85" s="3"/>
@@ -2169,7 +2237,7 @@
         <v>6.1728E-3</v>
       </c>
       <c r="E86">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>8.1000518403317781</v>
       </c>
       <c r="F86" s="3"/>
@@ -2185,7 +2253,7 @@
         <v>9.0909000000000007E-3</v>
       </c>
       <c r="E87">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>5.5000055000054999</v>
       </c>
       <c r="F87" s="3"/>
@@ -2201,7 +2269,7 @@
         <v>6.7568000000000003E-3</v>
       </c>
       <c r="E88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>7.399952640303102</v>
       </c>
       <c r="F88" s="3"/>
@@ -2217,7 +2285,7 @@
         <v>3.0303000000000001E-3</v>
       </c>
       <c r="E89">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>16.5000165000165</v>
       </c>
       <c r="F89" s="6"/>
@@ -2233,7 +2301,7 @@
         <v>8.4034000000000001E-3</v>
       </c>
       <c r="E90">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>5.9499726301259015</v>
       </c>
       <c r="F90" s="6"/>
@@ -2249,7 +2317,7 @@
         <v>8.3333000000000001E-3</v>
       </c>
       <c r="E91">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>6.0000240000960003</v>
       </c>
       <c r="F91" s="6"/>
@@ -2296,14 +2364,14 @@
         <v>7.5757999999999997E-3</v>
       </c>
       <c r="F93" s="6">
-        <f t="shared" ref="F93:F103" si="7">0.05/C93</f>
+        <f t="shared" ref="F93:F103" si="6">0.05/C93</f>
         <v>6.5999630402069753</v>
       </c>
       <c r="G93">
         <v>4.96</v>
       </c>
       <c r="I93">
-        <f t="shared" ref="I93:I103" si="8">G93/F93</f>
+        <f t="shared" ref="I93:I103" si="7">G93/F93</f>
         <v>0.75151935999999997</v>
       </c>
       <c r="J93">
@@ -2321,14 +2389,14 @@
         <v>5.0761000000000001E-3</v>
       </c>
       <c r="F94" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>9.8500817556785734</v>
       </c>
       <c r="G94">
         <v>5.5111111111111111</v>
       </c>
       <c r="I94">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.55949902222222214</v>
       </c>
       <c r="J94">
@@ -2346,14 +2414,14 @@
         <v>7.7518999999999999E-3</v>
       </c>
       <c r="F95" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>6.4500316051548658</v>
       </c>
       <c r="G95">
         <v>5.2044444444444444</v>
       </c>
       <c r="I95">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.80688665777777768</v>
       </c>
       <c r="J95">
@@ -2371,14 +2439,14 @@
         <v>7.9365000000000008E-3</v>
       </c>
       <c r="F96" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>6.3000063000062996</v>
       </c>
       <c r="G96">
         <v>4.0333333333333332</v>
       </c>
       <c r="I96">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.64021099999999997</v>
       </c>
       <c r="J96">
@@ -2396,14 +2464,14 @@
         <v>8.6957000000000007E-3</v>
       </c>
       <c r="F97" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>5.7499683751739363</v>
       </c>
       <c r="G97">
         <v>4.1288888888888886</v>
       </c>
       <c r="I97">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.71807158222222223</v>
       </c>
       <c r="J97">
@@ -2421,14 +2489,14 @@
         <v>6.6224999999999999E-3</v>
       </c>
       <c r="F98" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>7.5500188750471882</v>
       </c>
       <c r="G98">
         <v>4.1933333333333334</v>
       </c>
       <c r="I98">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.55540699999999998</v>
       </c>
       <c r="J98">
@@ -2446,14 +2514,14 @@
         <v>1.2194999999999999E-2</v>
       </c>
       <c r="F99" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>4.1000410004100045</v>
       </c>
       <c r="G99">
         <v>4.1266666666666669</v>
       </c>
       <c r="I99">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1.006494</v>
       </c>
       <c r="J99">
@@ -2471,14 +2539,14 @@
         <v>3.9215999999999999E-3</v>
       </c>
       <c r="F100" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>12.749898000815994</v>
       </c>
       <c r="G100">
         <v>4.3133333333333335</v>
       </c>
       <c r="I100">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.33830336</v>
       </c>
       <c r="J100">
@@ -2496,14 +2564,14 @@
         <v>1.1627999999999999E-2</v>
       </c>
       <c r="F101" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>4.2999656002751978</v>
       </c>
       <c r="G101">
         <v>1.5733333333333333</v>
       </c>
       <c r="I101">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.36589439999999995</v>
       </c>
       <c r="J101">
@@ -2521,14 +2589,14 @@
         <v>3.5971000000000002E-3</v>
       </c>
       <c r="F102" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>13.90008618053432</v>
       </c>
       <c r="G102">
         <v>5.0177777777777779</v>
       </c>
       <c r="I102">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.36098896888888887</v>
       </c>
       <c r="J102">
@@ -2546,14 +2614,14 @@
         <v>1.1627999999999999E-2</v>
       </c>
       <c r="F103" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>4.2999656002751978</v>
       </c>
       <c r="G103">
         <v>1.6311111111111112</v>
       </c>
       <c r="I103">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.37933120000000004</v>
       </c>
       <c r="J103">

</xml_diff>

<commit_message>
added some data viz to compare to hieu's data
</commit_message>
<xml_diff>
--- a/ptxdiffconc.xlsx
+++ b/ptxdiffconc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Feroze\Google Drive\DUKE 2016-2020\AxoSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E332405A-C6F2-40A7-87DF-0756C8AF2AA4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57028A7A-00AE-42B4-B54F-243BFB6D1F37}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="7932" xr2:uid="{7C8E119D-E43A-48DC-A79E-D87DB8623B38}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="241">
   <si>
     <t>Amplitude</t>
   </si>
@@ -726,6 +726,33 @@
   </si>
   <si>
     <t>PERCENT DIFFERENCE</t>
+  </si>
+  <si>
+    <t>concentration</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>1 nM</t>
+  </si>
+  <si>
+    <t>10 nM</t>
+  </si>
+  <si>
+    <t>100 nM</t>
+  </si>
+  <si>
+    <t>200 nM</t>
+  </si>
+  <si>
+    <t>400 nM</t>
+  </si>
+  <si>
+    <t>600 nM</t>
+  </si>
+  <si>
+    <t>1 uM</t>
   </si>
 </sst>
 </file>
@@ -817,6 +844,1091 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$211</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>mine</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Sheet1!$A$212:$A$219</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>control</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1 nM</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10 nM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100 nM</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200 nM</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>400 nM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>600 nM</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1 uM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$212:$B$219</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.32755025782733127</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.28893679346876028</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.28434407153268776</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25428759114555766</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.21515075636351677</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-60FE-4080-8894-32CDED2ADADF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$211</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>hieu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Sheet1!$A$212:$A$219</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>control</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1 nM</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10 nM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100 nM</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200 nM</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>400 nM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>600 nM</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1 uM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$212:$C$219</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.34280664588812804</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.26637512893996512</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2837454231523443</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.23645434888433103</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.27946602893331035</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-60FE-4080-8894-32CDED2ADADF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="695026032"/>
+        <c:axId val="695026360"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="695026032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="@" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="695026360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="695026360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="695026032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>944880</xdr:colOff>
+      <xdr:row>219</xdr:row>
+      <xdr:rowOff>127635</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>234</xdr:row>
+      <xdr:rowOff>127635</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A5BC98A-D9BE-41A9-8A05-7C32DD26E724}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1116,10 +2228,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69CF060E-16C0-45EF-9C8D-C01CC13BD142}">
-  <dimension ref="A1:X204"/>
+  <dimension ref="A1:X219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="E185" sqref="E185"/>
+    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
+      <selection activeCell="C212" sqref="C212:C219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5439,7 +6551,113 @@
         <v>0.217</v>
       </c>
     </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A210" s="7" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A211" t="s">
+        <v>232</v>
+      </c>
+      <c r="B211" t="s">
+        <v>229</v>
+      </c>
+      <c r="C211" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A212" t="s">
+        <v>233</v>
+      </c>
+      <c r="B212">
+        <v>0.32755025782733127</v>
+      </c>
+      <c r="C212">
+        <v>0.34280664588812804</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A213" t="s">
+        <v>234</v>
+      </c>
+      <c r="B213">
+        <v>0.28893679346876028</v>
+      </c>
+      <c r="C213">
+        <v>0.26637512893996512</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A214" t="s">
+        <v>235</v>
+      </c>
+      <c r="B214">
+        <v>0.28434407153268776</v>
+      </c>
+      <c r="C214">
+        <v>0.2837454231523443</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A215" t="s">
+        <v>236</v>
+      </c>
+      <c r="B215">
+        <v>0.25428759114555766</v>
+      </c>
+      <c r="C215">
+        <v>0.23645434888433103</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A216" t="s">
+        <v>237</v>
+      </c>
+      <c r="B216">
+        <v>0.21515075636351677</v>
+      </c>
+      <c r="C216">
+        <v>0.27946602893331035</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A217" t="s">
+        <v>238</v>
+      </c>
+      <c r="B217">
+        <v>0</v>
+      </c>
+      <c r="C217">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A218" t="s">
+        <v>239</v>
+      </c>
+      <c r="B218">
+        <v>0</v>
+      </c>
+      <c r="C218">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A219" t="s">
+        <v>240</v>
+      </c>
+      <c r="B219">
+        <v>0</v>
+      </c>
+      <c r="C219">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>